<commit_message>
modified by Roseline on 2025-06-03 23:54:17
</commit_message>
<xml_diff>
--- a/TenderScrap/TenderScrap/spiders/advert.xlsx
+++ b/TenderScrap/TenderScrap/spiders/advert.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -506,8 +510,12 @@
           <t>MAINTENANCE OF RAILWAY TRACK WITH ON-TRACK HIGH PRODUCTION BALLAST TAMPING MACHINES COUNTRYWIDE ON AN 'AS AND WHEN” REQUIRED' BASIS.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" s="2" t="n">
+        <v>45811.84238425926</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45828.5</v>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
@@ -516,7 +524,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97688</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97688</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -556,8 +564,12 @@
           <t>FOR THE PROVISION OF SUPPLY AND DELIVERY OF ICT CONSUMABLES</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="C3" s="2" t="n">
+        <v>45811.78873842592</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>6/6/2025 11:00:00 AM</t>
@@ -570,7 +582,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97687</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97687</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -611,8 +623,12 @@
 </t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="C4" s="2" t="n">
+        <v>45811.6865625</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -625,7 +641,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97549</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97549</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -665,8 +681,12 @@
           <t>RCB 06/2025/05	Land situated on Sub 21 (of 8) of Lot 5333, Umhlathuzi Lot 3/7,RBH 86-A-663</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="C5" s="2" t="n">
+        <v>45811.68482638889</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -679,7 +699,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97548</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97548</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -720,8 +740,12 @@
 </t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="C6" s="2" t="n">
+        <v>45811.68445601852</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -734,7 +758,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97546</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97546</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -774,8 +798,12 @@
           <t>RCB 06/2025/02 Land situated on Lot 3/4 Umhlathuzi sites, Bayview Precinct, RBH 86-A-689</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="C7" s="2" t="n">
+        <v>45811.6837037037</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -788,7 +816,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97544</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97544</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -828,8 +856,12 @@
           <t xml:space="preserve">FOR THE PROVISION OF THE SUPPLY AND INSTALLATION OF SUMP PUMPS; FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE PORT OF DURBAN: MAYDON WHARF AND AGRIPORT TERMINALS </t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="C8" s="2" t="n">
+        <v>45811.67271990741</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>6/10/2025 11:00:00 AM</t>
@@ -842,7 +874,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97651</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97651</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -882,8 +914,12 @@
           <t xml:space="preserve">SUPPLY OF PARTICIPANT GEAR FOR THE TPT NATIONAL AND GROUP SAFETY PROFICIENCY PROGRAMME </t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="C9" s="2" t="n">
+        <v>45811.67030092593</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
@@ -892,7 +928,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97652</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97652</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -932,8 +968,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF ENCODER; INCREMENTAL, 50 MM, AT THE CAPE TOWN CONTAINER TERMINAL AS ONCE OFF</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="C10" s="2" t="n">
+        <v>45811.6684375</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45814.66666666666</v>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
@@ -942,7 +982,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97666</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97666</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -982,8 +1022,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF STORE MAINTENANCE PARTS AT CAPE TOWN TERMINAL AS A ONCE-OFF PERIOD.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="C11" s="2" t="n">
+        <v>45811.65332175926</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45814.58333333334</v>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
@@ -992,7 +1036,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97644</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97644</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1032,8 +1076,12 @@
           <t>RCB 06/2025/11 Land situated on Lot 2/7 and 2/8 Umhlatuzi sites, Bayview Precinct</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="C12" s="2" t="n">
+        <v>45811.65217592593</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -1046,7 +1094,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97540</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97540</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1088,8 +1136,12 @@
 </t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="C13" s="2" t="n">
+        <v>45811.65131944444</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -1102,7 +1154,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97542</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97542</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1142,8 +1194,12 @@
           <t>RCB 06/2025/07	Land Situated on Newark Road, Bayview precinct, RBH 87-A-6020</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="C14" s="2" t="n">
+        <v>45811.64928240741</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -1156,7 +1212,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97552</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97552</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1196,8 +1252,12 @@
           <t>RCB 06/2025/09	Land Situated in Sub 21 (of 8) of Lot 5333, Umhlathuzi lot 2/6, RBH 86-A-682</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="C15" s="2" t="n">
+        <v>45811.64877314815</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -1210,7 +1270,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97555</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97555</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1250,8 +1310,12 @@
           <t>RCB 06/2025/10	Water area Walk-on Moorings and slipway, New Ark Precinct, RBH-89-A-646</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="C16" s="2" t="n">
+        <v>45811.64552083334</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>6/12/2025 9:00:00 AM</t>
@@ -1264,7 +1328,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97556</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97556</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1304,8 +1368,12 @@
           <t>FOR THE APPOINTMENT OF A SERVICE PROVIDER TO REMOVE WASTE AND PROVIDE WASTE MANAGEMENT SERVICES IN THE GERMISTON PLANT &amp; CENTRAL CORRIDOR FOR A PERIOD OF THREE (3) YEARS</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+      <c r="C17" s="2" t="n">
+        <v>45811.645</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45833.625</v>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>6/12/2025 10:00:00 AM</t>
@@ -1318,7 +1386,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97530</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97530</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1360,8 +1428,12 @@
 </t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="C18" s="2" t="n">
+        <v>45811.58258101852</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
           <t>6/10/2025 10:00:00 AM</t>
@@ -1374,7 +1446,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=93623</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/93623</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1414,8 +1486,12 @@
           <t xml:space="preserve">FOR THE PROVISION OF MOBILE CRANE HIRE FOR QC03 ,QC04 AND QC05  AT PIER 1 CONTAINER TERMINAL FOR PERIOD OF ONE DAY </t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="C19" s="2" t="n">
+        <v>45811.52672453703</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
@@ -1424,7 +1500,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97595</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97595</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1464,8 +1540,12 @@
           <t>FOR THE PROVISION OF BHEKULWANDLE LIBRARY WINDOWS AT PIER 1 CONTAINER TERMINAL</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="C20" s="2" t="n">
+        <v>45811.52664351852</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
           <t>6/10/2025 10:00:00 AM</t>
@@ -1478,7 +1558,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97601</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97601</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1518,8 +1598,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES .</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="C21" s="2" t="n">
+        <v>45811.52626157407</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
@@ -1528,7 +1612,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97622</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97622</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1568,8 +1652,12 @@
           <t>FOR THE ERADICATION OF ALIEN INVASIVE PLANTS AND PEST CONTROL</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="C22" s="2" t="n">
+        <v>45811.52148148148</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
@@ -1578,7 +1666,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97631</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97631</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1618,8 +1706,12 @@
           <t>FOR THE SUPPLY, DELIVERY AND RENTAL OF PERWAY AND WELDING TOOLS AT ERMELO FOR THE PERIOD OF SIX (6) MONTHS</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="C23" s="2" t="n">
+        <v>45811.44056712963</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>45826.41666666666</v>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
@@ -1628,7 +1720,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97612</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97612</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1668,8 +1760,12 @@
           <t>FOR THE SUPPLY OF BRAKE;EMERGENCY,240 KN,HOIST AND BOOM TO DURBAN CONTAINER TERMINAL PIER 2</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="C24" s="2" t="n">
+        <v>45810.64641203704</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
@@ -1678,7 +1774,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97534</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97534</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1718,8 +1814,12 @@
           <t>FOR THE SUPPLY OF VARIOUS STOCK ITEMS TO DURBAN CONTAINER TERMINAL PIER 2</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="C25" s="2" t="n">
+        <v>45810.64615740741</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
@@ -1728,7 +1828,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97551</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97551</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1768,8 +1868,12 @@
           <t>FOR THE PROVISION OF STATUTORY INSPECTION AIR RECEIVER AND STATUTORY INSPECTION TIPPLER 2 FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS AT THE PORT OF RICHARDS BAY.</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="C26" s="2" t="n">
+        <v>45810.61916666666</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
@@ -1778,7 +1882,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97537</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97537</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1818,8 +1922,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="C27" s="2" t="n">
+        <v>45810.58803240741</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
@@ -1828,7 +1936,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97524</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97524</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1868,8 +1976,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="C28" s="2" t="n">
+        <v>45810.58788194445</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
@@ -1878,7 +1990,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97520</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97520</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1918,8 +2030,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="C29" s="2" t="n">
+        <v>45810.56768518518</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
@@ -1928,7 +2044,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97516</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97516</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1968,8 +2084,12 @@
           <t>FOR THE PROVISION AND DELIVERY OF HIGH AND MEDIUM PRODUCTION BALLAST TAMPERS FOR COAL ANNUAL SHUTDOWN</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="C30" s="2" t="n">
+        <v>45810.5594212963</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45825.41666666666</v>
+      </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
@@ -1978,7 +2098,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97514</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97514</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2018,8 +2138,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="C31" s="2" t="n">
+        <v>45810.55778935185</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
@@ -2028,7 +2152,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97513</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97513</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2068,8 +2192,12 @@
           <t>HIRE 12 BAR MOBILE AIR COMPRESSOR</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+      <c r="C32" s="2" t="n">
+        <v>45810.54626157408</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>45812.5</v>
+      </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
@@ -2078,7 +2206,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97510</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97510</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2118,8 +2246,12 @@
           <t xml:space="preserve">FOR THE PROVISION OF REPAIR 55 KW AC TROLLEY MOTORS AT PIER 1 CONTAINER TERMINAL </t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="C33" s="2" t="n">
+        <v>45810.54322916667</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
@@ -2128,7 +2260,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97476</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97476</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2169,8 +2301,12 @@
 </t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="C34" s="2" t="n">
+        <v>45810.5203125</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>45819.5</v>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>6/6/2025 10:00:00 AM</t>
@@ -2183,7 +2319,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97473</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97473</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2223,8 +2359,12 @@
           <t>THE PROVISION TO RE-INSTATE OHTE INFRASTRUCTURE BETWEEN RUSTENBURG AND THABAZIMBI</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="C35" s="2" t="n">
+        <v>45810.44561342592</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>45825.41666666666</v>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
           <t>6/10/2025 11:00:00 AM</t>
@@ -2237,7 +2377,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97467</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97467</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2277,8 +2417,12 @@
           <t>FOR THE SUPPLY &amp; DELIVERY OF BATTERIES FOR TRANSNET SOC LTD (REG. NO 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE DURBAN CONTAINER TERMINAL (PIER 1 AND 2) ON AN AS AND WHEN BASIS FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="C36" s="2" t="n">
+        <v>45810.34425925926</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>45826.41666666666</v>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
@@ -2287,7 +2431,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97443</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97443</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2327,8 +2471,12 @@
           <t>FOR THE PROVISION OF CANTEEN AND CATERING SERVICES FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE NGQURA CONTAINER TERMINAL (NCT) AND PORT OF PORT ELIZABETH (PE)FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="C37" s="2" t="n">
+        <v>45807.66918981481</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>45835.95833333334</v>
+      </c>
       <c r="E37" t="inlineStr">
         <is>
           <t>6/18/2025 10:00:00 AM</t>
@@ -2341,7 +2489,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97428</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97428</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2381,8 +2529,12 @@
           <t>PROVISION OF HEAVY INDUSTRIAL PLANT CLEANING SERVICES FOR TRANSNET SOC LIMITED (REG. NO 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE BULK TERMINAL, PORT OF SALDANHA, FOR A PERIOD OF TWO (2) MONTHS.</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="C38" s="2" t="n">
+        <v>45807.65804398148</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>45812.54166666666</v>
+      </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
@@ -2391,7 +2543,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96710</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96710</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2431,8 +2583,12 @@
           <t>FOR THE  PROVISION OF A01, A02,A03 &amp; B GALLERY LIGHTING TO TRANSNET PORT TERMINAL IN RICHARDS BAY AS ONCE OFF.</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="C39" s="2" t="n">
+        <v>45807.63056712963</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>45819.5</v>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
           <t>6/4/2025 11:00:00 AM</t>
@@ -2445,7 +2601,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96781</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96781</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2485,8 +2641,12 @@
           <t>MANUFACTURE CABIN ACCESS PLATFORM</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+      <c r="C40" s="2" t="n">
+        <v>45807.62273148148</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
           <t>6/4/2025 10:00:00 AM</t>
@@ -2499,7 +2659,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97400</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97400</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2539,8 +2699,12 @@
           <t>FOR THE PROVISION OF TECHNICAL SERVICES ON A MIGRATION FROM SAP ECC6 TO SAP S/4HANA FOR TRANSNET CORPORATE CENTER (TCC) FOR A PERIOD OF TWELVE (12) MONTHS.</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="C41" s="2" t="n">
+        <v>45807.59373842592</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>45838.5</v>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
           <t>6/6/2025 11:00:00 AM</t>
@@ -2553,7 +2717,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=54684</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/54684</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2595,8 +2759,12 @@
 TRANSNET NATIONAL PORTS AUTHORITY IN THE PORT OF PORT ELIZABETH.</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
+      <c r="C42" s="2" t="n">
+        <v>45807.57770833333</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>45838.5</v>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
           <t>6/13/2025 12:00:00 PM</t>
@@ -2609,7 +2777,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97399</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97399</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2649,8 +2817,12 @@
           <t>PROVISION FOR THE REPAIRS AND MAINTENANCE OF WHARF FOREMAN FOR CIVIL MAINTENANCE DEPARTMENT AT THE PORT OF RICHARDS BAY FOR A PERIOD OF THREE (03) MONTHS</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="C43" s="2" t="n">
+        <v>45807.52611111111</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>45838.5</v>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
           <t>6/18/2025 10:00:00 AM</t>
@@ -2663,7 +2835,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94803</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94803</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2703,8 +2875,12 @@
           <t>Provision of service for Steelwork Repairs in the Port of East London</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="C44" s="2" t="n">
+        <v>45807.41094907407</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
@@ -2713,7 +2889,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97034</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97034</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2753,8 +2929,12 @@
           <t>FOR THE TEST AND REPAIR OF INTERNAL TRACTION TRANSFORMER FAULT AT TURFGROND AT, INFRA KOEDOESPOORT</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+      <c r="C45" s="2" t="n">
+        <v>45807.3596875</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>45819.41666666666</v>
+      </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
@@ -2763,7 +2943,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97327</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97327</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2803,8 +2983,12 @@
           <t>MAINTENANCE OF RAILWAY TRACK WITH ON-TRACK MEDIUM PRODUCTION UNIVERAL BALLAST TAMPING MACHINES AND A BALLAST STABILISER COUNTRYWIDE ON AN 'AS AND WHEN” REQUIRED' BASIS</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="C46" s="2" t="n">
+        <v>45807.33966435185</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>45821.41666666666</v>
+      </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
@@ -2813,7 +2997,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97328</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97328</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2854,8 +3038,12 @@
 PROVIDE, SERV;RECERTIFY,XB SAMPLE TEST</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+      <c r="C47" s="2" t="n">
+        <v>45806.6893287037</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>45820.75</v>
+      </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
@@ -2864,7 +3052,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97249</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97249</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2904,8 +3092,12 @@
           <t xml:space="preserve">REPAIR OF THE BOOM HYDRAULIC RAM 524 FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS AT THE DURBAN CONTAINER TERMINAL </t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="C48" s="2" t="n">
+        <v>45806.63712962963</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
           <t>6/2/2025 10:00:00 AM</t>
@@ -2918,7 +3110,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97251</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97251</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2958,8 +3150,12 @@
           <t>REPLACEMENT AND INSTALLATION OF FENCE AT THE PORT OF NGQURA AND COEGA KOP QUARRY FOR A PERIOD OF TEN (10) MONTH</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
+      <c r="C49" s="2" t="n">
+        <v>45806.62247685185</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>45838.625</v>
+      </c>
       <c r="E49" t="inlineStr">
         <is>
           <t>6/11/2025 10:00:00 AM</t>
@@ -2972,7 +3168,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94422</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94422</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3012,8 +3208,12 @@
           <t>REQUEST FOR PROVISION OF SERVICE TO SUPPLY AND DELIVER RO PLANT HIGH PRESSURE FEED PUMP.</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+      <c r="C50" s="2" t="n">
+        <v>45806.55134259259</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>45812.83333333334</v>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
           <t>6/2/2025 11:00:00 AM</t>
@@ -3026,7 +3226,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97097</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97097</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3068,8 +3268,12 @@
 TRACTION SUBSTATIONS UNDER THE CONTROL OF DEPOT ENGINEER.</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="C51" s="2" t="n">
+        <v>45806.51459490741</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>45821.41666666666</v>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
           <t>6/6/2025 10:00:00 AM</t>
@@ -3082,7 +3286,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97240</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97240</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3122,8 +3326,12 @@
           <t>HEALTH AND SAFETY AGENT/S ON THE PORT ELIZABETH (PE) FOR CIVIL BULK INFRASTRUCTURE UPGRADE (FOR A PERIOD OF THIRTY-SIX (36) MONTHS) AND/OR MARINE INFRASTRUCTURE UPGRADE (FOR A PERIOD OF TWENTY-FOUR (24) MONTHS) AND/OR NATIONAL FIRE SERVICES INFRASTRUCTURE EQUIPMENT UPGRADE PHASE 2A  (FOR A PERIOD OF FIFTEEN (15) MONTHS)</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="C52" s="2" t="n">
+        <v>45806.48064814815</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>45827.5</v>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
           <t>6/5/2025 10:00:00 AM</t>
@@ -3136,7 +3344,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=89905</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/89905</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -3176,8 +3384,12 @@
           <t>THE APPOINTMENT OF A PROFESSIONAL SERVICE PROVIDER FOR THE BOEGOEBAAI PORT AND RAIL DEVELOPMENT MARKET RESEARCH STUDIES FOR A PERIOD OF SIX (6) MONTHS</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+      <c r="C53" s="2" t="n">
+        <v>45806.45256944445</v>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>45835.66666666666</v>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
           <t>6/6/2025 10:00:00 AM</t>
@@ -3190,7 +3402,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92645</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92645</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3230,8 +3442,12 @@
           <t>FOR THE PROVISION OF REPAIRS TO WASH BAY ROOF &amp; HAULER WORKSHOP BUILDING</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="C54" s="2" t="n">
+        <v>45806.4412962963</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E54" t="inlineStr">
         <is>
           <t>6/10/2025 10:00:00 AM</t>
@@ -3244,7 +3460,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97217</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97217</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3284,8 +3500,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF XV, XN AND XB WAGONS SAFETY RELIEF VALVES FOR TRANSNET ENGINEERING, FOR GERMISTON AND BLOEMFONTEIN ON AN “AS AND WHEN” REQUIRED BASIS FOR A PERIOD OF FIVE (5) YEARS</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
+      <c r="C55" s="2" t="n">
+        <v>45806.38208333333</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E55" t="inlineStr">
         <is>
           <t>6/11/2025 11:00:00 AM</t>
@@ -3298,7 +3518,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97214</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97214</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3338,8 +3558,12 @@
           <t>RFP REQUEST FOR THE PROVISION OF DRY DOCK MAINTENANCE OF THE LAUNCH KITE, PILOT BOAT AVOCET, WORK BOAT CRESTED TERN, TUG OSPREY, TUG CORMORANT, TUG JUTTEN/LOTHENI AND TUG CHARDONNAY FOR TRANSNET NATIONAL PORTS AUTHORITY (TNPA), PORT OF SALDANHA, ON AN AS AND WHEN REQUIRED BASIS FOR A PERIOD OF THIRTY-SIX (36) MONTHS</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
+      <c r="C56" s="2" t="n">
+        <v>45806.37510416667</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>45832.58333333334</v>
+      </c>
       <c r="E56" t="inlineStr">
         <is>
           <t>6/10/2025 11:00:00 AM</t>
@@ -3352,7 +3576,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=80674</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/80674</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3392,8 +3616,12 @@
           <t>For an appointment of a publishing house to wholly develop, publish, print and distribute one Magazine for a period of (3) Three years</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
+      <c r="C57" s="2" t="n">
+        <v>45805.73349537037</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>45826.5</v>
+      </c>
       <c r="E57" t="inlineStr">
         <is>
           <t>6/5/2025 11:00:00 AM</t>
@@ -3406,7 +3634,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=91127</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/91127</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -3446,8 +3674,12 @@
           <t>For the Provision of Roof Repairs and General Building Maintenance Services at the ex-Transtel building at TNPA in the Port of Richards Bay for a period of four (4) months.</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" s="2" t="n">
+        <v>45805.58128472222</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>45820.5</v>
+      </c>
       <c r="E58" t="inlineStr">
         <is>
           <t>6/5/2025 10:00:00 AM</t>
@@ -3460,7 +3692,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=93883</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/93883</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3500,8 +3732,12 @@
           <t>LAB CONSUMABLES</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" s="2" t="n">
+        <v>45805.36445601852</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>45818.625</v>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
@@ -3510,7 +3746,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92732</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92732</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3550,8 +3786,12 @@
           <t>LAB MACHINE MAINTENANCE SERVICES</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
+      <c r="C60" s="2" t="n">
+        <v>45805.36417824074</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>45814.625</v>
+      </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
@@ -3560,7 +3800,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96993</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96993</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3600,8 +3840,12 @@
           <t>PROVISION OF OFFICE, BUILDING, WORKSHOP CLEANING AND TEA SERVICES FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE PORT OF DURBAN: MPT POINT, CAR TERMINAL, MAYDON WHARF AND AGRIBULK FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="C61" s="2" t="n">
+        <v>45804.70929398148</v>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>45819.41666666666</v>
+      </c>
       <c r="E61" t="inlineStr">
         <is>
           <t>6/3/2025 10:00:00 AM</t>
@@ -3614,7 +3858,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97073</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97073</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3655,8 +3899,12 @@
 EQUIPMENTS AND WELDER CERTIFICATION AT TRANSNET ENGINEERING, GERMISTON.</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="C62" s="2" t="n">
+        <v>45804.65201388889</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>45812.625</v>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
@@ -3665,7 +3913,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=97057</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/97057</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3705,8 +3953,12 @@
           <t>FOR THE PROVISION OF REPAIR, TESTING AND COMMISSIONING OF TWO RAIL-ROAD SHUNTING LOCOMOTIVES SALDANHA AT TRANSNET ENGINEERING FOR A ONCE-OFF PERIOD</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="C63" s="2" t="n">
+        <v>45804.58878472223</v>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>45833.45833333334</v>
+      </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
@@ -3715,7 +3967,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96968</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96968</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3757,8 +4009,12 @@
 CONVEYOR</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="C64" s="2" t="n">
+        <v>45804.47309027778</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>45818.66666666666</v>
+      </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
@@ -3767,7 +4023,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96985</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96985</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3807,8 +4063,12 @@
           <t>EXPRESSION OF INTEREST (EOI) REQUIRED IN RELATION TO TRIDEM AXLE BOGIE WITH OVERSLUNG SUSPENSION (TRAILER) FOR USE AT PORT TERMINAL, MARITIME BUSINESS, TRANSNET ENGINEERING, RICHARDS BAY.</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+      <c r="C65" s="2" t="n">
+        <v>45804.37309027778</v>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>45819.58333333334</v>
+      </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
@@ -3817,7 +4077,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=95158</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/95158</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3858,8 +4118,12 @@
 INFRASTRUCTURE MANAGER’S SECURITY DEPARTMENT.</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="C66" s="2" t="n">
+        <v>45804.32800925926</v>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>45832.54166666666</v>
+      </c>
       <c r="E66" t="inlineStr">
         <is>
           <t>6/3/2025 11:00:00 AM</t>
@@ -3872,7 +4136,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96953</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96953</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3912,8 +4176,12 @@
           <t xml:space="preserve"> PROVISION TO REFURBISHMENT OF SUBSTATION 1A AND 1B AT NGQURA CONTAINER TERMINAL FOR TRANSNET SOC LTD (REG NO:1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED AS “TPT”) FOR NGQURA CONTAINER TERMINAL AS A ONCE OFF </t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="C67" s="2" t="n">
+        <v>45803.6796875</v>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>45835.58333333334</v>
+      </c>
       <c r="E67" t="inlineStr">
         <is>
           <t>6/10/2025 11:00:00 AM</t>
@@ -3926,7 +4194,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96950</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96950</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -3968,8 +4236,12 @@
 MUNCHER</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="C68" s="2" t="n">
+        <v>45803.63376157408</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>45817.66666666666</v>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
@@ -3978,7 +4250,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96921</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96921</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -4018,8 +4290,12 @@
           <t>SUPPLY, INSTALLATION, COMMISSIONING AND TESTING OF NEW SMALL BASIC MINI-CNC LATHE MACHINE FOR PD BUSINESS AT KOEDOESPOORT FOR ONCE OFF PERIOD, AT TRANSNET ENGINEERING</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
+      <c r="C69" s="2" t="n">
+        <v>45803.56710648148</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>45813.58333333334</v>
+      </c>
       <c r="E69" t="inlineStr">
         <is>
           <t>5/30/2025 10:00:00 AM</t>
@@ -4032,7 +4308,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96841</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96841</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4076,8 +4352,12 @@
 </t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
+      <c r="C70" s="2" t="n">
+        <v>45803.54571759259</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E70" t="inlineStr">
         <is>
           <t>5/29/2025 10:00:00 AM</t>
@@ -4090,7 +4370,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96898</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96898</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -4130,8 +4410,12 @@
           <t>FOR THE SUPPLY, DELIVERY AND INSTALLATION OF STEEL PALISADE WITH ELECTRIC FENCE AT OGIES/ERMELO</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="C71" s="2" t="n">
+        <v>45803.47934027778</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>45817.41666666666</v>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
@@ -4140,7 +4424,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96878</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96878</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -4180,8 +4464,12 @@
           <t>PROVISION OF HYGIENE AND PEST CONTROL SERVICES AT SCHEEPERSNECK FOR 24 MONTHS PERIOD</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="C72" s="2" t="n">
+        <v>45803.36966435185</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>45813.45833333334</v>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
           <t>5/30/2025 11:00:00 AM</t>
@@ -4194,7 +4482,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96672</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96672</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -4234,8 +4522,12 @@
           <t xml:space="preserve">FOR THE MAINTENANCE OF RAILWAY TRACK WITH AN ON-TRACK HIGH PRODUCTION SCREENING MACHINE ON ALL LINES OWNED AND MAINTAINED BY TRANSNET </t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
+      <c r="C73" s="2" t="n">
+        <v>45803.32575231481</v>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
@@ -4244,7 +4536,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96842</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96842</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -4284,8 +4576,12 @@
           <t>PROVISION OF COMPREHENSIVE SCAFFOLDING SERVICES ON AN AS AND WHEN REQUIRED BASIS FOR A PERIOD OF 2 MONTHS FOR TRANSNET PORT TERMINALS RICHARDS BAY</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+      <c r="C74" s="2" t="n">
+        <v>45800.67446759259</v>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>45814.58333333334</v>
+      </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
@@ -4294,7 +4590,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96670</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96670</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -4335,8 +4631,12 @@
 RECON, COMP;DRAWGEAR KEYSTONE</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
+      <c r="C75" s="2" t="n">
+        <v>45800.63063657407</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>45818.75</v>
+      </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
@@ -4345,7 +4645,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=95898</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/95898</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -4385,8 +4685,12 @@
           <t>FOR THE PROVISION OF MAINTENANCE FOR RAIL DISPATCH BUILDING TARLTON DEPOT ON A ONCE OFF BASIS</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
+      <c r="C76" s="2" t="n">
+        <v>45800.53383101852</v>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>45817.66666666666</v>
+      </c>
       <c r="E76" t="inlineStr">
         <is>
           <t>6/2/2025 11:00:00 AM</t>
@@ -4399,7 +4703,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=88724</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/88724</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4440,8 +4744,12 @@
 </t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
+      <c r="C77" s="2" t="n">
+        <v>45800.5280324074</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
@@ -4450,7 +4758,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96729</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96729</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -4490,8 +4798,12 @@
           <t xml:space="preserve">PROVISION OF S04 TAIL STRUCTURAL REPAIRS </t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
+      <c r="C78" s="2" t="n">
+        <v>45800.51077546296</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>45814.33333333334</v>
+      </c>
       <c r="E78" t="inlineStr">
         <is>
           <t>5/30/2025 10:00:00 AM</t>
@@ -4504,7 +4816,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96661</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96661</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4544,8 +4856,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF SOAPS AND DETERGENTS TRANSNET SOC LTD REG. NO. 1990/000900) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) FOR THE DURBAN CONTAINER TERMINALS PIER 1 AND PIER 2. FOR A PERIOD OF THIRTY-SIX MONTHS (36) MONTHS.</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
+      <c r="C79" s="2" t="n">
+        <v>45800.50451388889</v>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
@@ -4554,7 +4870,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96770</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96770</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -4594,8 +4910,12 @@
           <t>THE PROVISION OF AN ACCREDITED YOUNG LEADERS PROGRAMME WITHIN TRANSNET, FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="C80" s="2" t="n">
+        <v>45800.47005787037</v>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>45835.66666666666</v>
+      </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
@@ -4604,7 +4924,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96361</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96361</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -4644,8 +4964,12 @@
           <t>REPAIR DAMAGED LEAKING ROOFS WITHIN THE RM BUSINESS WORKSHOP 150 EEL ROAD UMBILO</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="C81" s="2" t="n">
+        <v>45800.44152777778</v>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>45817.54166666666</v>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
           <t>6/3/2025 11:00:00 AM</t>
@@ -4658,7 +4982,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96663</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96663</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -4698,8 +5022,12 @@
           <t>FOR THE PROVISION OF WASTE REMOVAL SERVICES IN NORTHERN KZN (EMPANGENI, RICHARDS BAY AND VRYHEID AND SURROUNDING AREAS) FOR TRANSNET PROPERTY FOR A PERIOD OF THIRTY SIX (36) MONTHS</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+      <c r="C82" s="2" t="n">
+        <v>45799.79829861111</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E82" t="inlineStr">
         <is>
           <t>5/29/2025 9:30:00 AM</t>
@@ -4712,7 +5040,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=93373</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/93373</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -4752,8 +5080,12 @@
           <t xml:space="preserve">PROVISION OF PEST CONTROL SERVICES AT VRYHEID, EMPANGENI , RICHARDS BAY AND SURROUNDING AREAS FOR TRANSNET PROPERTY FOR A PERIOD OF 36 MONTHS. </t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+      <c r="C83" s="2" t="n">
+        <v>45799.79804398148</v>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>45821.58333333334</v>
+      </c>
       <c r="E83" t="inlineStr">
         <is>
           <t>5/29/2025 11:00:00 AM</t>
@@ -4766,7 +5098,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94085</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94085</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -4806,8 +5138,12 @@
           <t>FOR THE APPOINTMENT OF A SERVICE PROVIDER TO CONDUCT INTERNAL SHOTBLAST FOR RAIL TANKS AT TRANSNET ENGINEERING, GERMISTON DEPOT ON AN AS AND WHEN BASIS FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
+      <c r="C84" s="2" t="n">
+        <v>45799.65636574074</v>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>45813.66666666666</v>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
           <t>5/29/2025 11:00:00 AM</t>
@@ -4820,7 +5156,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96693</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96693</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -4860,8 +5196,12 @@
           <t>SUPPLY, INSTALLATION AND MOULDING HDPE PIPES FOR INTERMEDIATE PUMPS FOR TRANSNET PORT TERMINAL - RICHARDS BAY - AS A ONCE OFF SERVICE</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
+      <c r="C85" s="2" t="n">
+        <v>45799.50821759259</v>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>45814.58333333334</v>
+      </c>
       <c r="E85" t="inlineStr">
         <is>
           <t>5/30/2025 11:00:00 AM</t>
@@ -4874,7 +5214,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96578</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96578</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -4914,8 +5254,12 @@
           <t>THE PROVISION OF INSPECTION AND CALIBRATION SERVICES FOR PRESSURE RELIEF DEVICES AT VARIOUS TRANSNET PIPELINES SITES FOR A PERIOD OF FOUR (4) YEARS.</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
+      <c r="C86" s="2" t="n">
+        <v>45798.73452546296</v>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E86" t="inlineStr">
         <is>
           <t>5/30/2025 10:00:00 AM</t>
@@ -4928,7 +5272,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92507</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92507</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -4968,8 +5312,12 @@
           <t>FOR THE APPOINTMENT OF FINANCIAL INSTITUTION(S) TO ACT AS LEAD ARRANGER(S) AND TRANSACTION ADVISOR(S) FOR SPECIFIC ISSUANCES UNDER TRANSNET’S R80 BILLION DOMESTIC MEDIUM-TERM NOTE (“DMTN”) PROGRAMME FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
+      <c r="C87" s="2" t="n">
+        <v>45798.68741898148</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>45821.66666666666</v>
+      </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
@@ -4978,7 +5326,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94467</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94467</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -5018,8 +5366,12 @@
           <t>Provision of service for the maintenance, repair and installation (if necessary) of air conditioning units in Kimberley South relay rooms (Spuitfontein to De Aar) as and when required for a period of two (2) years.</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="C88" s="2" t="n">
+        <v>45798.6144212963</v>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>45825.41666666666</v>
+      </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
@@ -5028,7 +5380,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96567</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96567</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -5069,8 +5421,12 @@
 </t>
         </is>
       </c>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
+      <c r="C89" s="2" t="n">
+        <v>45797.47945601852</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
@@ -5079,7 +5435,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=63385</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/63385</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -5119,8 +5475,12 @@
           <t xml:space="preserve"> CIDB - FOR THE PROVISION TO REPAIR THE CONCRETE STRUCTURE FOR GP4 SHED FOR TRANSNET SOC LTD</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
+      <c r="C90" s="2" t="n">
+        <v>45796.62003472223</v>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>45814.54166666666</v>
+      </c>
       <c r="E90" t="inlineStr">
         <is>
           <t>5/26/2025 10:00:00 AM</t>
@@ -5133,7 +5493,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96253</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96253</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -5175,8 +5535,12 @@
 </t>
         </is>
       </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
+      <c r="C91" s="2" t="n">
+        <v>45794.54615740741</v>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>45812.58333333334</v>
+      </c>
       <c r="E91" t="inlineStr">
         <is>
           <t>5/19/2025 11:00:00 AM</t>
@@ -5189,7 +5553,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96243</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96243</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -5229,8 +5593,12 @@
           <t>FOR THE SUPPLY, DELIVERY, INSTALLATION, TESTING AND COMMISSIONING OF 9 OFF ROTARY SCREW TYPE COMPRESSORS AND AIR DRYERS FOR TRANSNET ENGINEERING AT VARIOUS CORRIDOR DEPOTS (NORTH CAPE AND CONTAINER CORRIDORS)</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
+      <c r="C92" s="2" t="n">
+        <v>45793.60487268519</v>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>45818.5</v>
+      </c>
       <c r="E92" t="inlineStr">
         <is>
           <t>5/26/2025 9:30:00 AM</t>
@@ -5243,7 +5611,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94658</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94658</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -5283,8 +5651,12 @@
           <t>FOR THE PROVISION OF NETWORK DETECTION AND RESPONSE (NDR) SOLUTION FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="C93" s="2" t="n">
+        <v>45793.48670138889</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>45827.5</v>
+      </c>
       <c r="E93" t="inlineStr">
         <is>
           <t>5/23/2025 11:00:00 AM</t>
@@ -5297,7 +5669,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=84866</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/84866</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -5338,8 +5710,12 @@
 </t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="C94" s="2" t="n">
+        <v>45792.64659722222</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>45838.75</v>
+      </c>
       <c r="E94" t="inlineStr">
         <is>
           <t>5/27/2025 10:00:00 AM</t>
@@ -5352,7 +5728,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=96000</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/96000</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -5392,8 +5768,12 @@
           <t>SUPPLY AND DELIVERY OF VARIOUS AMOUR ROCK FOR THE CONSTRUCTION WORK IN THE UPGRADE OF THE BREAKWATERS (NEW DOLOSSE) AT THE PORT OF RICHARDS BAY</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
+      <c r="C95" s="2" t="n">
+        <v>45792.61826388889</v>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>45817.66666666666</v>
+      </c>
       <c r="E95" t="inlineStr">
         <is>
           <t>5/26/2025 10:00:00 AM</t>
@@ -5406,7 +5786,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=90555</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/90555</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -5446,8 +5826,12 @@
           <t>THE ESTABLISHMENT OF AN  APPROVED LIST OF SERVICE PROVIDERS FOR PROVISION OF LEGAL SERVICES FOR A PERIOD OF FIVE (5) YEARS</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
+      <c r="C96" s="2" t="n">
+        <v>45791.66534722222</v>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E96" t="inlineStr">
         <is>
           <t>5/23/2024 11:00:00 AM</t>
@@ -5460,7 +5844,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=65599</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/65599</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5501,8 +5885,12 @@
 </t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
+      <c r="C97" s="2" t="n">
+        <v>45791.47337962963</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>45821.75</v>
+      </c>
       <c r="E97" t="inlineStr">
         <is>
           <t>5/19/2025 1:00:00 PM</t>
@@ -5515,7 +5903,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94921</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94921</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -5559,8 +5947,12 @@
 </t>
         </is>
       </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
+      <c r="C98" s="2" t="n">
+        <v>45790.86484953704</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>45814.41666666666</v>
+      </c>
       <c r="E98" t="inlineStr">
         <is>
           <t>5/22/2025 10:00:00 AM</t>
@@ -5573,7 +5965,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=95751</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/95751</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -5613,8 +6005,12 @@
           <t>FOR THE DESIGN, MANUFACTURE, OFF SITE TESTING, SUPPLY, DELIVERY, INSTALLATION, TESTING AND COMMISSIONING OF ONE (1) NEW 1000KVA MINI SUBSTATION AND ONE (1) 1000KVA MOBILE GENERATOR FOR THE ENGINEERING EQUIPMENT SERVICES (EES) BUILDING, FOR TRANSNET SOC LTD OPERATING AS TRANSNET PORT TERMINALS, (HEREINAFTER REFERRED TO AS “TPT”), AT DURBAN CONTAINER TERMINAL PIER 1, FOR THE DURATION OF 12 MONTHS</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
+      <c r="C99" s="2" t="n">
+        <v>45790.62701388889</v>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>45817</v>
+      </c>
       <c r="E99" t="inlineStr">
         <is>
           <t>5/21/2025 12:00:00 AM</t>
@@ -5627,7 +6023,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=95844</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/95844</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -5667,8 +6063,12 @@
           <t>MECHANICAL UPGRADE AT SASOLBURG DIESEL STORAGE DEPOT, FREE STATE.</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="C100" s="2" t="n">
+        <v>45789.69364583334</v>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>45821.41666666666</v>
+      </c>
       <c r="E100" t="inlineStr">
         <is>
           <t>5/22/2025 10:12:00 AM</t>
@@ -5681,7 +6081,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=95743</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/95743</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -5721,8 +6121,12 @@
           <t xml:space="preserve">THE DESIGN, SUPPLY, DELIVERY, INSTALLATION, TESTING AND COMMISSIONING OF A COMPLETE NEW SHOT BLAST BOOTH INCLUDING THE STRUCTURE FOR THE LOCOMOTIVE BUSINESS DURBAN FOR A PERIOD OF FOUR (04) MONTHS. </t>
         </is>
       </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="C101" s="2" t="n">
+        <v>45786.61042824074</v>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>45814.75</v>
+      </c>
       <c r="E101" t="inlineStr">
         <is>
           <t>5/19/2025 11:00:00 AM</t>
@@ -5735,7 +6139,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94930</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94930</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -5775,8 +6179,12 @@
           <t>FOR A SERVICE PROVIDER TO PROVIDE THE SERVICES OF AN APPROVED INSPECTION AUTHORITY (AIA) TO CONDUCT SAMPLE TESTING ON THE XB WAGONS FLEET IN LINE WITH SPECIFICATION EW_KLP_SPEC_2003 IN BLOEMFONTEIN ON AN “AS AND WHEN” REQUIRED BASIS FOR A PERIOD OF FOUR (4) YEARS.</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+      <c r="C102" s="2" t="n">
+        <v>45785.36899305556</v>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>45814.66666666666</v>
+      </c>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr">
         <is>
@@ -5785,7 +6193,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=91624</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/91624</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -5825,8 +6233,12 @@
           <t>FOR AN APPOINTMENT OF A SERVICE PROVIDER TO OPERATE  AND  TAKE OVER OWNERSHIP SCHOOL OF EXCELLENCE</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
+      <c r="C103" s="2" t="n">
+        <v>45784.35107638889</v>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>45821.625</v>
+      </c>
       <c r="E103" t="inlineStr">
         <is>
           <t>5/21/2025 11:00:00 AM</t>
@@ -5839,7 +6251,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92369</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92369</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -5879,8 +6291,12 @@
           <t>FOR THE APPOINTMENT OF A REGISTERED PROFESSIONAL TO PERFORM AN EPC ASSESSMENT, MEASUREMENT OF THE BUILDING NET FLOOR AREA AND ENERGY DATA ON 13 FACILITIES TO TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE VARIOUS TRANSNET PORT TERMINALS ON A ONCE OFF BASIS.</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
+      <c r="C104" s="2" t="n">
+        <v>45783.49142361111</v>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E104" t="inlineStr">
         <is>
           <t>5/16/2025 11:00:00 AM</t>
@@ -5893,7 +6309,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92515</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92515</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -5933,8 +6349,12 @@
           <t>DESIGN, SUPPLY, DELIVER AND CONSTRUCT THE PERIMETER FENCE WITH INTRUSION DETECTION AT UITENHAGE (SWARTKOPS), FOR A PERIOD OF 06 MONTHS</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
+      <c r="C105" s="2" t="n">
+        <v>45782.56052083334</v>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>45817.75</v>
+      </c>
       <c r="E105" t="inlineStr">
         <is>
           <t>5/13/2025 10:00:00 AM</t>
@@ -5947,7 +6367,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92908</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92908</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -5987,8 +6407,12 @@
           <t>FOR THE LEASE AND/OR DEVELOPMENT OF THE REMAINDER OF ERF 34104 BELLVILLE (UNREGISTERED SUBDIVISION OF REMAINDER OF ERF 11661 BELLVILLE), ERF 34103 BELLVILLE (UNREGISTERED SUBDIVISION OF REMAINDER OF ERF 11659 BELLVILLE), ERF 22933 PAROW.</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
+      <c r="C106" s="2" t="n">
+        <v>45780.34752314815</v>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>45838.95833333334</v>
+      </c>
       <c r="E106" t="inlineStr">
         <is>
           <t>5/19/2025 11:00:00 AM</t>
@@ -6001,7 +6425,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92763</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92763</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6041,8 +6465,12 @@
           <t>DECOMMISSIONING OF OBSOLETE NETWORK VIDEO RECORDERS (NVRs), SUPPLY, INSTALLATION, CONFIGURATION, INTEGRATION, TRAINING, MAINTENANCE, AND COMMISSIONING OF A NEW NVR AND SOFTWARE FOR THE CCTV SURVEILLANCE SYSTEM AT KILNERPARK CORPORATE OFFICE FOR A PERIOD OF 12 MONTHS</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+      <c r="C107" s="2" t="n">
+        <v>45777.94576388889</v>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>45818.41666666666</v>
+      </c>
       <c r="E107" t="inlineStr">
         <is>
           <t>5/14/2025 11:00:00 AM</t>
@@ -6055,7 +6483,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94967</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94967</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -6095,8 +6523,12 @@
           <t>FOR THE SUPPLY, INSTALLATION, AND COMMISSIONING OF SHOP 5 WORKSHOP EQUIPMENT/MACHINERY AT THE DRY BULK TERMINAL PORT OF RICHARDS BAY WORKS FOR TRANSNET SOC LTD OPERATING AS TRANSNET PORT TERMINALS</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
+      <c r="C108" s="2" t="n">
+        <v>45764.48126157407</v>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>45812.5</v>
+      </c>
       <c r="E108" t="inlineStr">
         <is>
           <t>5/6/2025 11:00:00 AM</t>
@@ -6109,7 +6541,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=94230</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/94230</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -6149,8 +6581,12 @@
           <t>DESIGN, SUPPLY, INSTALLATION (EPC CONTRACTOR) AND PROVIDE PLANNED MAINTENANCE FOR A LIMITED PERIOD FOR THE VAPOUR RECOVERY UNIT SYSTEM AT THE TPL TARLTON PETROLEUM PRODUCTS HANDLING AND BULK STORAGE FACILITY</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr"/>
+      <c r="C109" s="2" t="n">
+        <v>45763.49534722222</v>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>45814.625</v>
+      </c>
       <c r="E109" t="inlineStr">
         <is>
           <t>4/25/2025 11:00:00 AM</t>
@@ -6163,7 +6599,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=70943</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/70943</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -6203,8 +6639,12 @@
           <t>REQUEST FOR PROPOSALS FOR THE APPOINTMENT OF A TERMINAL OPERATOR TO FINANCE, DESIGN, CONSTRUCT, OPERATE, MAINTAIN, AND TRANSFER A MULTI-PURPOSE TERMINAL HANDLING FRESH PRODUCE AND COMPATIBLE BREAK BULK CARGO FOR A TWENTY-FIVE (25) YEAR CONCESSION PERIOD AT MAYDON WHARF PRECINCT IN THE PORT OF DURBAN.</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="C110" s="2" t="n">
+        <v>45758.65010416666</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>45898.66666666666</v>
+      </c>
       <c r="E110" t="inlineStr">
         <is>
           <t>5/7/2025 10:00:00 AM</t>
@@ -6217,7 +6657,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=93866</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/93866</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -6257,8 +6697,12 @@
           <t>Request for Qualification (RFQ) for the Establishment of the Rolling Stock Leasing Company (LeaseCo) for Transnet SOC Ltd operating as Transnet Corporate Centre</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr"/>
+      <c r="C111" s="2" t="n">
+        <v>45755.66251157408</v>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>45842.66666666666</v>
+      </c>
       <c r="E111" t="inlineStr">
         <is>
           <t>5/6/2025 11:00:00 AM</t>
@@ -6271,7 +6715,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=92339</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/92339</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -6311,8 +6755,12 @@
           <t>APPOINTMENT OF A TERMINAL OPERATOR TO ACQUIRE, OPERATE, MAINTAIN, REFURBISH, AND/OR CONSTRUCT AND TRANSFER A LIQUID BULK TERMINAL FOR A TWENTY-FIVE (25) YEAR CONCESSION PERIOD AT THE PORT OF CAPE TOWN LIQUID BULK PRECINCT</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+      <c r="C112" s="2" t="n">
+        <v>45750.64232638889</v>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>45881.66666666666</v>
+      </c>
       <c r="E112" t="inlineStr">
         <is>
           <t>4/17/2025 10:00:00 AM</t>
@@ -6325,7 +6773,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=90040</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/90040</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -6366,8 +6814,12 @@
 CONVEYOR SOLUTION FOR TRANSNET SOC (REG. N0 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS RICHARDS BAY (HEREINAFTER REFERRED TO AS “TPT RCB”)</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
+      <c r="C113" s="2" t="n">
+        <v>45743.61306712963</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>45838.41666666666</v>
+      </c>
       <c r="E113" t="inlineStr">
         <is>
           <t>4/10/2025 10:00:00 AM</t>
@@ -6380,7 +6832,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=85636</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/85636</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -6420,8 +6872,12 @@
           <t>REQUEST FOR PROPOSAL FOR THE APPOINTMENT OF A TERMINAL OPERATOR TO FINANCE, DESIGN, CONSTRUCT, OPERATE, MAINTAIN, AND TRANSFER A MULTI-PURPOSE TERMINAL HANDLING AGRICULTURAL DRY BULK AND OTHER COMPATIBLE CARGO FOR A TWENTY-FIVE (25) YEAR CONCESSION PERIOD AT MAYDON WHARF PRECINCT AT THE PORT OF DURBAN.</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr"/>
+      <c r="C114" s="2" t="n">
+        <v>45723.59657407407</v>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>45849.66666666666</v>
+      </c>
       <c r="E114" t="inlineStr">
         <is>
           <t>3/27/2025 10:00:00 AM</t>
@@ -6434,7 +6890,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>https://transnetetenders.azurewebsites.net/Home/TenderDetails?Id=90945</t>
+          <t>https://publishedetenders.blob.core.windows.net/publishedetenderscontainer/90945</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">

</xml_diff>

<commit_message>
modified by Roseline on 2025-06-03 23:56:37
</commit_message>
<xml_diff>
--- a/TenderScrap/TenderScrap/spiders/advert.xlsx
+++ b/TenderScrap/TenderScrap/spiders/advert.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -558,10 +562,8 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6/6/2025 11:00:00 AM</t>
-        </is>
+      <c r="E3" s="2" t="n">
+        <v>45814.45833333334</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -613,10 +615,8 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E4" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -667,10 +667,8 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E5" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -722,10 +720,8 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E6" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -776,10 +772,8 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E7" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -830,10 +824,8 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>6/10/2025 11:00:00 AM</t>
-        </is>
+      <c r="E8" s="2" t="n">
+        <v>45818.45833333334</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1034,10 +1026,8 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E12" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1090,10 +1080,8 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E13" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1144,10 +1132,8 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E14" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1198,10 +1184,8 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E15" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1252,10 +1236,8 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>6/12/2025 9:00:00 AM</t>
-        </is>
+      <c r="E16" s="2" t="n">
+        <v>45820.375</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1306,10 +1288,8 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>6/12/2025 10:00:00 AM</t>
-        </is>
+      <c r="E17" s="2" t="n">
+        <v>45820.41666666666</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1362,10 +1342,8 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>6/10/2025 10:00:00 AM</t>
-        </is>
+      <c r="E18" s="2" t="n">
+        <v>45818.41666666666</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1466,10 +1444,8 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>6/10/2025 10:00:00 AM</t>
-        </is>
+      <c r="E20" s="2" t="n">
+        <v>45818.41666666666</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2171,10 +2147,8 @@
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>6/6/2025 10:00:00 AM</t>
-        </is>
+      <c r="E34" s="2" t="n">
+        <v>45814.41666666666</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2225,10 +2199,8 @@
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>6/10/2025 11:00:00 AM</t>
-        </is>
+      <c r="E35" s="2" t="n">
+        <v>45818.45833333334</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2329,10 +2301,8 @@
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>6/18/2025 10:00:00 AM</t>
-        </is>
+      <c r="E37" s="2" t="n">
+        <v>45826.41666666666</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -2433,10 +2403,8 @@
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>6/4/2025 11:00:00 AM</t>
-        </is>
+      <c r="E39" s="2" t="n">
+        <v>45812.45833333334</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -2487,10 +2455,8 @@
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>6/4/2025 10:00:00 AM</t>
-        </is>
+      <c r="E40" s="2" t="n">
+        <v>45812.41666666666</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2541,10 +2507,8 @@
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>6/6/2025 11:00:00 AM</t>
-        </is>
+      <c r="E41" s="2" t="n">
+        <v>45814.45833333334</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2597,10 +2561,8 @@
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>6/13/2025 12:00:00 PM</t>
-        </is>
+      <c r="E42" s="2" t="n">
+        <v>45821.5</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2651,10 +2613,8 @@
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>6/18/2025 10:00:00 AM</t>
-        </is>
+      <c r="E43" s="2" t="n">
+        <v>45826.41666666666</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2906,10 +2866,8 @@
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>6/2/2025 10:00:00 AM</t>
-        </is>
+      <c r="E48" s="2" t="n">
+        <v>45810.41666666666</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2960,10 +2918,8 @@
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>6/11/2025 10:00:00 AM</t>
-        </is>
+      <c r="E49" s="2" t="n">
+        <v>45819.41666666666</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -3014,10 +2970,8 @@
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>6/2/2025 11:00:00 AM</t>
-        </is>
+      <c r="E50" s="2" t="n">
+        <v>45810.45833333334</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3070,10 +3024,8 @@
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>6/6/2025 10:00:00 AM</t>
-        </is>
+      <c r="E51" s="2" t="n">
+        <v>45814.41666666666</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -3124,10 +3076,8 @@
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>6/5/2025 10:00:00 AM</t>
-        </is>
+      <c r="E52" s="2" t="n">
+        <v>45813.41666666666</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -3178,10 +3128,8 @@
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>6/6/2025 10:00:00 AM</t>
-        </is>
+      <c r="E53" s="2" t="n">
+        <v>45814.41666666666</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -3232,10 +3180,8 @@
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>6/10/2025 10:00:00 AM</t>
-        </is>
+      <c r="E54" s="2" t="n">
+        <v>45818.41666666666</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -3286,10 +3232,8 @@
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>6/11/2025 11:00:00 AM</t>
-        </is>
+      <c r="E55" s="2" t="n">
+        <v>45819.45833333334</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -3340,10 +3284,8 @@
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>6/10/2025 11:00:00 AM</t>
-        </is>
+      <c r="E56" s="2" t="n">
+        <v>45818.45833333334</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -3394,10 +3336,8 @@
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>6/5/2025 11:00:00 AM</t>
-        </is>
+      <c r="E57" s="2" t="n">
+        <v>45813.45833333334</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -3448,10 +3388,8 @@
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>6/5/2025 10:00:00 AM</t>
-        </is>
+      <c r="E58" s="2" t="n">
+        <v>45813.41666666666</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -3602,10 +3540,8 @@
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>6/3/2025 10:00:00 AM</t>
-        </is>
+      <c r="E61" s="2" t="n">
+        <v>45811.41666666666</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -3860,10 +3796,8 @@
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>6/3/2025 11:00:00 AM</t>
-        </is>
+      <c r="E66" s="2" t="n">
+        <v>45811.45833333334</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -3914,10 +3848,8 @@
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>6/10/2025 11:00:00 AM</t>
-        </is>
+      <c r="E67" s="2" t="n">
+        <v>45818.45833333334</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -4020,10 +3952,8 @@
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>5/30/2025 10:00:00 AM</t>
-        </is>
+      <c r="E69" s="2" t="n">
+        <v>45807.41666666666</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -4078,10 +4008,8 @@
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>5/29/2025 10:00:00 AM</t>
-        </is>
+      <c r="E70" s="2" t="n">
+        <v>45806.41666666666</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -4182,10 +4110,8 @@
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>5/30/2025 11:00:00 AM</t>
-        </is>
+      <c r="E72" s="2" t="n">
+        <v>45807.45833333334</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -4387,10 +4313,8 @@
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>6/2/2025 11:00:00 AM</t>
-        </is>
+      <c r="E76" s="2" t="n">
+        <v>45810.45833333334</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -4492,10 +4416,8 @@
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>5/30/2025 10:00:00 AM</t>
-        </is>
+      <c r="E78" s="2" t="n">
+        <v>45807.41666666666</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -4646,10 +4568,8 @@
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>6/3/2025 11:00:00 AM</t>
-        </is>
+      <c r="E81" s="2" t="n">
+        <v>45811.45833333334</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -4700,10 +4620,8 @@
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>5/29/2025 9:30:00 AM</t>
-        </is>
+      <c r="E82" s="2" t="n">
+        <v>45806.39583333334</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -4754,10 +4672,8 @@
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>5/29/2025 11:00:00 AM</t>
-        </is>
+      <c r="E83" s="2" t="n">
+        <v>45806.45833333334</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -4808,10 +4724,8 @@
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>5/29/2025 11:00:00 AM</t>
-        </is>
+      <c r="E84" s="2" t="n">
+        <v>45806.45833333334</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -4862,10 +4776,8 @@
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>5/30/2025 11:00:00 AM</t>
-        </is>
+      <c r="E85" s="2" t="n">
+        <v>45807.45833333334</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -4916,10 +4828,8 @@
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>5/30/2025 10:00:00 AM</t>
-        </is>
+      <c r="E86" s="2" t="n">
+        <v>45807.41666666666</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -5121,10 +5031,8 @@
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>5/26/2025 10:00:00 AM</t>
-        </is>
+      <c r="E90" s="2" t="n">
+        <v>45803.41666666666</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -5177,10 +5085,8 @@
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>5/19/2025 11:00:00 AM</t>
-        </is>
+      <c r="E91" s="2" t="n">
+        <v>45796.45833333334</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -5231,10 +5137,8 @@
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>5/26/2025 9:30:00 AM</t>
-        </is>
+      <c r="E92" s="2" t="n">
+        <v>45803.39583333334</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -5285,10 +5189,8 @@
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>5/23/2025 11:00:00 AM</t>
-        </is>
+      <c r="E93" s="2" t="n">
+        <v>45800.45833333334</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -5340,10 +5242,8 @@
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>5/27/2025 10:00:00 AM</t>
-        </is>
+      <c r="E94" s="2" t="n">
+        <v>45804.41666666666</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -5394,10 +5294,8 @@
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>5/26/2025 10:00:00 AM</t>
-        </is>
+      <c r="E95" s="2" t="n">
+        <v>45803.41666666666</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -5448,10 +5346,8 @@
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>5/23/2024 11:00:00 AM</t>
-        </is>
+      <c r="E96" s="2" t="n">
+        <v>45435.45833333334</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -5503,10 +5399,8 @@
       </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>5/19/2025 1:00:00 PM</t>
-        </is>
+      <c r="E97" s="2" t="n">
+        <v>45796.54166666666</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
@@ -5561,10 +5455,8 @@
       </c>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>5/22/2025 10:00:00 AM</t>
-        </is>
+      <c r="E98" s="2" t="n">
+        <v>45799.41666666666</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -5615,10 +5507,8 @@
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>5/21/2025 12:00:00 AM</t>
-        </is>
+      <c r="E99" s="2" t="n">
+        <v>45798</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -5669,10 +5559,8 @@
       </c>
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr"/>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>5/22/2025 10:12:00 AM</t>
-        </is>
+      <c r="E100" s="2" t="n">
+        <v>45799.425</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -5723,10 +5611,8 @@
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>5/19/2025 11:00:00 AM</t>
-        </is>
+      <c r="E101" s="2" t="n">
+        <v>45796.45833333334</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -5827,10 +5713,8 @@
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>5/21/2025 11:00:00 AM</t>
-        </is>
+      <c r="E103" s="2" t="n">
+        <v>45798.45833333334</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -5881,10 +5765,8 @@
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>5/16/2025 11:00:00 AM</t>
-        </is>
+      <c r="E104" s="2" t="n">
+        <v>45793.45833333334</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -5935,10 +5817,8 @@
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>5/13/2025 10:00:00 AM</t>
-        </is>
+      <c r="E105" s="2" t="n">
+        <v>45790.41666666666</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -5989,10 +5869,8 @@
       </c>
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>5/19/2025 11:00:00 AM</t>
-        </is>
+      <c r="E106" s="2" t="n">
+        <v>45796.45833333334</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -6043,10 +5921,8 @@
       </c>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>5/14/2025 11:00:00 AM</t>
-        </is>
+      <c r="E107" s="2" t="n">
+        <v>45791.45833333334</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
@@ -6097,10 +5973,8 @@
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>5/6/2025 11:00:00 AM</t>
-        </is>
+      <c r="E108" s="2" t="n">
+        <v>45783.45833333334</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -6151,10 +6025,8 @@
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>4/25/2025 11:00:00 AM</t>
-        </is>
+      <c r="E109" s="2" t="n">
+        <v>45772.45833333334</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -6205,10 +6077,8 @@
       </c>
       <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr"/>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>5/7/2025 10:00:00 AM</t>
-        </is>
+      <c r="E110" s="2" t="n">
+        <v>45784.41666666666</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -6259,10 +6129,8 @@
       </c>
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr"/>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>5/6/2025 11:00:00 AM</t>
-        </is>
+      <c r="E111" s="2" t="n">
+        <v>45783.45833333334</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -6313,10 +6181,8 @@
       </c>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>4/17/2025 10:00:00 AM</t>
-        </is>
+      <c r="E112" s="2" t="n">
+        <v>45764.41666666666</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -6368,10 +6234,8 @@
       </c>
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>4/10/2025 10:00:00 AM</t>
-        </is>
+      <c r="E113" s="2" t="n">
+        <v>45757.41666666666</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -6422,10 +6286,8 @@
       </c>
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>3/27/2025 10:00:00 AM</t>
-        </is>
+      <c r="E114" s="2" t="n">
+        <v>45743.41666666666</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
modified by Roseline on 2025-06-03 23:57:58
</commit_message>
<xml_diff>
--- a/TenderScrap/TenderScrap/spiders/advert.xlsx
+++ b/TenderScrap/TenderScrap/spiders/advert.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -562,8 +558,10 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" s="2" t="n">
-        <v>45814.45833333334</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-06-06 11:00:00</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -615,8 +613,10 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -667,8 +667,10 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -720,8 +722,10 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -772,8 +776,10 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -824,8 +830,10 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" s="2" t="n">
-        <v>45818.45833333334</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:00:00</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1026,8 +1034,10 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1080,8 +1090,10 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1132,8 +1144,10 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1184,8 +1198,10 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1236,8 +1252,10 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" s="2" t="n">
-        <v>45820.375</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-06-12 09:00:00</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1288,8 +1306,10 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" s="2" t="n">
-        <v>45820.41666666666</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-06-12 10:00:00</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1342,8 +1362,10 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" s="2" t="n">
-        <v>45818.41666666666</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-06-10 10:00:00</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1444,8 +1466,10 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" s="2" t="n">
-        <v>45818.41666666666</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-06-10 10:00:00</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2147,8 +2171,10 @@
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" s="2" t="n">
-        <v>45814.41666666666</v>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2025-06-06 10:00:00</t>
+        </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2199,8 +2225,10 @@
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" s="2" t="n">
-        <v>45818.45833333334</v>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:00:00</t>
+        </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2301,8 +2329,10 @@
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" s="2" t="n">
-        <v>45826.41666666666</v>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2025-06-18 10:00:00</t>
+        </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -2403,8 +2433,10 @@
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" s="2" t="n">
-        <v>45812.45833333334</v>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-06-04 11:00:00</t>
+        </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -2455,8 +2487,10 @@
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" s="2" t="n">
-        <v>45812.41666666666</v>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-06-04 10:00:00</t>
+        </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2507,8 +2541,10 @@
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
-      <c r="E41" s="2" t="n">
-        <v>45814.45833333334</v>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-06-06 11:00:00</t>
+        </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2561,8 +2597,10 @@
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" s="2" t="n">
-        <v>45821.5</v>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2025-06-13 12:00:00</t>
+        </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2613,8 +2651,10 @@
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" s="2" t="n">
-        <v>45826.41666666666</v>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2025-06-18 10:00:00</t>
+        </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2866,8 +2906,10 @@
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" s="2" t="n">
-        <v>45810.41666666666</v>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2025-06-02 10:00:00</t>
+        </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2918,8 +2960,10 @@
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" s="2" t="n">
-        <v>45819.41666666666</v>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2025-06-11 10:00:00</t>
+        </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2970,8 +3014,10 @@
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" s="2" t="n">
-        <v>45810.45833333334</v>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2025-06-02 11:00:00</t>
+        </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3024,8 +3070,10 @@
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
-      <c r="E51" s="2" t="n">
-        <v>45814.41666666666</v>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2025-06-06 10:00:00</t>
+        </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -3076,8 +3124,10 @@
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
-      <c r="E52" s="2" t="n">
-        <v>45813.41666666666</v>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2025-06-05 10:00:00</t>
+        </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -3128,8 +3178,10 @@
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
-      <c r="E53" s="2" t="n">
-        <v>45814.41666666666</v>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2025-06-06 10:00:00</t>
+        </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -3180,8 +3232,10 @@
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
-      <c r="E54" s="2" t="n">
-        <v>45818.41666666666</v>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2025-06-10 10:00:00</t>
+        </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -3232,8 +3286,10 @@
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" s="2" t="n">
-        <v>45819.45833333334</v>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2025-06-11 11:00:00</t>
+        </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -3284,8 +3340,10 @@
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
-      <c r="E56" s="2" t="n">
-        <v>45818.45833333334</v>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:00:00</t>
+        </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -3336,8 +3394,10 @@
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" s="2" t="n">
-        <v>45813.45833333334</v>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-06-05 11:00:00</t>
+        </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -3388,8 +3448,10 @@
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
-      <c r="E58" s="2" t="n">
-        <v>45813.41666666666</v>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-06-05 10:00:00</t>
+        </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -3540,8 +3602,10 @@
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
-      <c r="E61" s="2" t="n">
-        <v>45811.41666666666</v>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-06-03 10:00:00</t>
+        </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -3796,8 +3860,10 @@
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
-      <c r="E66" s="2" t="n">
-        <v>45811.45833333334</v>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-06-03 11:00:00</t>
+        </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -3848,8 +3914,10 @@
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
-      <c r="E67" s="2" t="n">
-        <v>45818.45833333334</v>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-06-10 11:00:00</t>
+        </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -3952,8 +4020,10 @@
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
-      <c r="E69" s="2" t="n">
-        <v>45807.41666666666</v>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2025-05-30 10:00:00</t>
+        </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -4008,8 +4078,10 @@
       </c>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
-      <c r="E70" s="2" t="n">
-        <v>45806.41666666666</v>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2025-05-29 10:00:00</t>
+        </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -4110,8 +4182,10 @@
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" s="2" t="n">
-        <v>45807.45833333334</v>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>2025-05-30 11:00:00</t>
+        </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -4313,8 +4387,10 @@
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" s="2" t="n">
-        <v>45810.45833333334</v>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>2025-06-02 11:00:00</t>
+        </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -4416,8 +4492,10 @@
       </c>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" s="2" t="n">
-        <v>45807.41666666666</v>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2025-05-30 10:00:00</t>
+        </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -4568,8 +4646,10 @@
       </c>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" s="2" t="n">
-        <v>45811.45833333334</v>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>2025-06-03 11:00:00</t>
+        </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -4620,8 +4700,10 @@
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
-      <c r="E82" s="2" t="n">
-        <v>45806.39583333334</v>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2025-05-29 09:30:00</t>
+        </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -4672,8 +4754,10 @@
       </c>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" s="2" t="n">
-        <v>45806.45833333334</v>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>2025-05-29 11:00:00</t>
+        </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -4724,8 +4808,10 @@
       </c>
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
-      <c r="E84" s="2" t="n">
-        <v>45806.45833333334</v>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>2025-05-29 11:00:00</t>
+        </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -4776,8 +4862,10 @@
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" s="2" t="n">
-        <v>45807.45833333334</v>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>2025-05-30 11:00:00</t>
+        </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -4828,8 +4916,10 @@
       </c>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
-      <c r="E86" s="2" t="n">
-        <v>45807.41666666666</v>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>2025-05-30 10:00:00</t>
+        </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -5031,8 +5121,10 @@
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
-      <c r="E90" s="2" t="n">
-        <v>45803.41666666666</v>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>2025-05-26 10:00:00</t>
+        </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -5085,8 +5177,10 @@
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
-      <c r="E91" s="2" t="n">
-        <v>45796.45833333334</v>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>2025-05-19 11:00:00</t>
+        </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -5137,8 +5231,10 @@
       </c>
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr"/>
-      <c r="E92" s="2" t="n">
-        <v>45803.39583333334</v>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2025-05-26 09:30:00</t>
+        </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -5189,8 +5285,10 @@
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr"/>
-      <c r="E93" s="2" t="n">
-        <v>45800.45833333334</v>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2025-05-23 11:00:00</t>
+        </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -5242,8 +5340,10 @@
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
-      <c r="E94" s="2" t="n">
-        <v>45804.41666666666</v>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>2025-05-27 10:00:00</t>
+        </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -5294,8 +5394,10 @@
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr"/>
-      <c r="E95" s="2" t="n">
-        <v>45803.41666666666</v>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>2025-05-26 10:00:00</t>
+        </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -5346,8 +5448,10 @@
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr"/>
-      <c r="E96" s="2" t="n">
-        <v>45435.45833333334</v>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>2024-05-23 11:00:00</t>
+        </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -5399,8 +5503,10 @@
       </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
-      <c r="E97" s="2" t="n">
-        <v>45796.54166666666</v>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>2025-05-19 13:00:00</t>
+        </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
@@ -5455,8 +5561,10 @@
       </c>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
-      <c r="E98" s="2" t="n">
-        <v>45799.41666666666</v>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>2025-05-22 10:00:00</t>
+        </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -5507,8 +5615,10 @@
       </c>
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr"/>
-      <c r="E99" s="2" t="n">
-        <v>45798</v>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>2025-05-21 00:00:00</t>
+        </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -5559,8 +5669,10 @@
       </c>
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr"/>
-      <c r="E100" s="2" t="n">
-        <v>45799.425</v>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>2025-05-22 10:12:00</t>
+        </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -5611,8 +5723,10 @@
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr"/>
-      <c r="E101" s="2" t="n">
-        <v>45796.45833333334</v>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>2025-05-19 11:00:00</t>
+        </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -5713,8 +5827,10 @@
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr"/>
-      <c r="E103" s="2" t="n">
-        <v>45798.45833333334</v>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2025-05-21 11:00:00</t>
+        </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -5765,8 +5881,10 @@
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
-      <c r="E104" s="2" t="n">
-        <v>45793.45833333334</v>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2025-05-16 11:00:00</t>
+        </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -5817,8 +5935,10 @@
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
-      <c r="E105" s="2" t="n">
-        <v>45790.41666666666</v>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2025-05-13 10:00:00</t>
+        </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -5869,8 +5989,10 @@
       </c>
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr"/>
-      <c r="E106" s="2" t="n">
-        <v>45796.45833333334</v>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2025-05-19 11:00:00</t>
+        </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -5921,8 +6043,10 @@
       </c>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr"/>
-      <c r="E107" s="2" t="n">
-        <v>45791.45833333334</v>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2025-05-14 11:00:00</t>
+        </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
@@ -5973,8 +6097,10 @@
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
-      <c r="E108" s="2" t="n">
-        <v>45783.45833333334</v>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2025-05-06 11:00:00</t>
+        </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -6025,8 +6151,10 @@
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr"/>
-      <c r="E109" s="2" t="n">
-        <v>45772.45833333334</v>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2025-04-25 11:00:00</t>
+        </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -6077,8 +6205,10 @@
       </c>
       <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr"/>
-      <c r="E110" s="2" t="n">
-        <v>45784.41666666666</v>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>2025-05-07 10:00:00</t>
+        </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -6129,8 +6259,10 @@
       </c>
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr"/>
-      <c r="E111" s="2" t="n">
-        <v>45783.45833333334</v>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2025-05-06 11:00:00</t>
+        </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -6181,8 +6313,10 @@
       </c>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
-      <c r="E112" s="2" t="n">
-        <v>45764.41666666666</v>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2025-04-17 10:00:00</t>
+        </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -6234,8 +6368,10 @@
       </c>
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
-      <c r="E113" s="2" t="n">
-        <v>45757.41666666666</v>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2025-04-10 10:00:00</t>
+        </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -6286,8 +6422,10 @@
       </c>
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr"/>
-      <c r="E114" s="2" t="n">
-        <v>45743.41666666666</v>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2025-03-27 10:00:00</t>
+        </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
modified by Roseline on 2025-06-04 00:17:59
</commit_message>
<xml_diff>
--- a/TenderScrap/TenderScrap/spiders/advert.xlsx
+++ b/TenderScrap/TenderScrap/spiders/advert.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -506,8 +510,12 @@
           <t>MAINTENANCE OF RAILWAY TRACK WITH ON-TRACK HIGH PRODUCTION BALLAST TAMPING MACHINES COUNTRYWIDE ON AN 'AS AND WHEN” REQUIRED' BASIS.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" s="2" t="n">
+        <v>45811.84238425926</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45828.5</v>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
@@ -556,11 +564,15 @@
           <t>FOR THE PROVISION OF SUPPLY AND DELIVERY OF ICT CONSUMABLES</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="C3" s="2" t="n">
+        <v>45811.78873842592</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-06-06 11:00:00</t>
+          <t>6/6/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -611,11 +623,15 @@
 </t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="C4" s="2" t="n">
+        <v>45811.6865625</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -665,11 +681,15 @@
           <t>RCB 06/2025/05	Land situated on Sub 21 (of 8) of Lot 5333, Umhlathuzi Lot 3/7,RBH 86-A-663</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="C5" s="2" t="n">
+        <v>45811.68482638889</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -720,11 +740,15 @@
 </t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="C6" s="2" t="n">
+        <v>45811.68445601852</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -774,11 +798,15 @@
           <t>RCB 06/2025/02 Land situated on Lot 3/4 Umhlathuzi sites, Bayview Precinct, RBH 86-A-689</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="C7" s="2" t="n">
+        <v>45811.6837037037</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -828,11 +856,15 @@
           <t xml:space="preserve">FOR THE PROVISION OF THE SUPPLY AND INSTALLATION OF SUMP PUMPS; FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE PORT OF DURBAN: MAYDON WHARF AND AGRIPORT TERMINALS </t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="C8" s="2" t="n">
+        <v>45811.67271990741</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-06-10 11:00:00</t>
+          <t>6/10/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -882,8 +914,12 @@
           <t xml:space="preserve">SUPPLY OF PARTICIPANT GEAR FOR THE TPT NATIONAL AND GROUP SAFETY PROFICIENCY PROGRAMME </t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="C9" s="2" t="n">
+        <v>45811.67030092593</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
@@ -932,8 +968,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF ENCODER; INCREMENTAL, 50 MM, AT THE CAPE TOWN CONTAINER TERMINAL AS ONCE OFF</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="C10" s="2" t="n">
+        <v>45811.6684375</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45814.66666666666</v>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
@@ -982,8 +1022,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF STORE MAINTENANCE PARTS AT CAPE TOWN TERMINAL AS A ONCE-OFF PERIOD.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="C11" s="2" t="n">
+        <v>45811.65332175926</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45814.58333333334</v>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
@@ -1032,11 +1076,15 @@
           <t>RCB 06/2025/11 Land situated on Lot 2/7 and 2/8 Umhlatuzi sites, Bayview Precinct</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="C12" s="2" t="n">
+        <v>45811.65217592593</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1088,11 +1136,15 @@
 </t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="C13" s="2" t="n">
+        <v>45811.65131944444</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1142,11 +1194,15 @@
           <t>RCB 06/2025/07	Land Situated on Newark Road, Bayview precinct, RBH 87-A-6020</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="C14" s="2" t="n">
+        <v>45811.64928240741</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1196,11 +1252,15 @@
           <t>RCB 06/2025/09	Land Situated in Sub 21 (of 8) of Lot 5333, Umhlathuzi lot 2/6, RBH 86-A-682</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="C15" s="2" t="n">
+        <v>45811.64877314815</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1250,11 +1310,15 @@
           <t>RCB 06/2025/10	Water area Walk-on Moorings and slipway, New Ark Precinct, RBH-89-A-646</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="C16" s="2" t="n">
+        <v>45811.64552083334</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00:00</t>
+          <t>6/12/2025 9:00:00 AM</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1304,11 +1368,15 @@
           <t>FOR THE APPOINTMENT OF A SERVICE PROVIDER TO REMOVE WASTE AND PROVIDE WASTE MANAGEMENT SERVICES IN THE GERMISTON PLANT &amp; CENTRAL CORRIDOR FOR A PERIOD OF THREE (3) YEARS</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+      <c r="C17" s="2" t="n">
+        <v>45811.645</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45833.625</v>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-06-12 10:00:00</t>
+          <t>6/12/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1360,11 +1428,15 @@
 </t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+      <c r="C18" s="2" t="n">
+        <v>45811.58258101852</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-06-10 10:00:00</t>
+          <t>6/10/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1414,8 +1486,12 @@
           <t xml:space="preserve">FOR THE PROVISION OF MOBILE CRANE HIRE FOR QC03 ,QC04 AND QC05  AT PIER 1 CONTAINER TERMINAL FOR PERIOD OF ONE DAY </t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+      <c r="C19" s="2" t="n">
+        <v>45811.52672453703</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
@@ -1464,11 +1540,15 @@
           <t>FOR THE PROVISION OF BHEKULWANDLE LIBRARY WINDOWS AT PIER 1 CONTAINER TERMINAL</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="C20" s="2" t="n">
+        <v>45811.52664351852</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-06-10 10:00:00</t>
+          <t>6/10/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1518,8 +1598,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES .</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="C21" s="2" t="n">
+        <v>45811.52626157407</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
@@ -1568,8 +1652,12 @@
           <t>FOR THE ERADICATION OF ALIEN INVASIVE PLANTS AND PEST CONTROL</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+      <c r="C22" s="2" t="n">
+        <v>45811.52148148148</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
@@ -1618,8 +1706,12 @@
           <t>FOR THE SUPPLY, DELIVERY AND RENTAL OF PERWAY AND WELDING TOOLS AT ERMELO FOR THE PERIOD OF SIX (6) MONTHS</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+      <c r="C23" s="2" t="n">
+        <v>45811.44056712963</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>45826.41666666666</v>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
@@ -1668,8 +1760,12 @@
           <t>FOR THE SUPPLY OF BRAKE;EMERGENCY,240 KN,HOIST AND BOOM TO DURBAN CONTAINER TERMINAL PIER 2</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="C24" s="2" t="n">
+        <v>45810.64641203704</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
@@ -1718,8 +1814,12 @@
           <t>FOR THE SUPPLY OF VARIOUS STOCK ITEMS TO DURBAN CONTAINER TERMINAL PIER 2</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+      <c r="C25" s="2" t="n">
+        <v>45810.64615740741</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
@@ -1768,8 +1868,12 @@
           <t>FOR THE PROVISION OF STATUTORY INSPECTION AIR RECEIVER AND STATUTORY INSPECTION TIPPLER 2 FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS AT THE PORT OF RICHARDS BAY.</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+      <c r="C26" s="2" t="n">
+        <v>45810.61916666666</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
@@ -1818,8 +1922,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="C27" s="2" t="n">
+        <v>45810.58803240741</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
@@ -1868,8 +1976,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="C28" s="2" t="n">
+        <v>45810.58788194445</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
@@ -1918,8 +2030,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="C29" s="2" t="n">
+        <v>45810.56768518518</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
@@ -1968,8 +2084,12 @@
           <t>FOR THE PROVISION AND DELIVERY OF HIGH AND MEDIUM PRODUCTION BALLAST TAMPERS FOR COAL ANNUAL SHUTDOWN</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+      <c r="C30" s="2" t="n">
+        <v>45810.5594212963</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45825.41666666666</v>
+      </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
@@ -2018,8 +2138,12 @@
           <t>SUPPLY OF VARIOUS ITEMS TO PIER ONE STORES.</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+      <c r="C31" s="2" t="n">
+        <v>45810.55778935185</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
@@ -2068,8 +2192,12 @@
           <t>HIRE 12 BAR MOBILE AIR COMPRESSOR</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
+      <c r="C32" s="2" t="n">
+        <v>45810.54626157408</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>45812.5</v>
+      </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
@@ -2118,8 +2246,12 @@
           <t xml:space="preserve">FOR THE PROVISION OF REPAIR 55 KW AC TROLLEY MOTORS AT PIER 1 CONTAINER TERMINAL </t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+      <c r="C33" s="2" t="n">
+        <v>45810.54322916667</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
@@ -2169,11 +2301,15 @@
 </t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="C34" s="2" t="n">
+        <v>45810.5203125</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>45819.5</v>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-06-06 10:00:00</t>
+          <t>6/6/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2223,11 +2359,15 @@
           <t>THE PROVISION TO RE-INSTATE OHTE INFRASTRUCTURE BETWEEN RUSTENBURG AND THABAZIMBI</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="C35" s="2" t="n">
+        <v>45810.44561342592</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>45825.41666666666</v>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-06-10 11:00:00</t>
+          <t>6/10/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2277,8 +2417,12 @@
           <t>FOR THE SUPPLY &amp; DELIVERY OF BATTERIES FOR TRANSNET SOC LTD (REG. NO 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE DURBAN CONTAINER TERMINAL (PIER 1 AND 2) ON AN AS AND WHEN BASIS FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="C36" s="2" t="n">
+        <v>45810.34425925926</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>45826.41666666666</v>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
@@ -2327,11 +2471,15 @@
           <t>FOR THE PROVISION OF CANTEEN AND CATERING SERVICES FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE NGQURA CONTAINER TERMINAL (NCT) AND PORT OF PORT ELIZABETH (PE)FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+      <c r="C37" s="2" t="n">
+        <v>45807.66918981481</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>45835.95833333334</v>
+      </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-06-18 10:00:00</t>
+          <t>6/18/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2381,8 +2529,12 @@
           <t>PROVISION OF HEAVY INDUSTRIAL PLANT CLEANING SERVICES FOR TRANSNET SOC LIMITED (REG. NO 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE BULK TERMINAL, PORT OF SALDANHA, FOR A PERIOD OF TWO (2) MONTHS.</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="C38" s="2" t="n">
+        <v>45807.65804398148</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>45812.54166666666</v>
+      </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
@@ -2431,11 +2583,15 @@
           <t>FOR THE  PROVISION OF A01, A02,A03 &amp; B GALLERY LIGHTING TO TRANSNET PORT TERMINAL IN RICHARDS BAY AS ONCE OFF.</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="C39" s="2" t="n">
+        <v>45807.63056712963</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>45819.5</v>
+      </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-06-04 11:00:00</t>
+          <t>6/4/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2485,11 +2641,15 @@
           <t>MANUFACTURE CABIN ACCESS PLATFORM</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
+      <c r="C40" s="2" t="n">
+        <v>45807.62273148148</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-06-04 10:00:00</t>
+          <t>6/4/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2539,11 +2699,15 @@
           <t>FOR THE PROVISION OF TECHNICAL SERVICES ON A MIGRATION FROM SAP ECC6 TO SAP S/4HANA FOR TRANSNET CORPORATE CENTER (TCC) FOR A PERIOD OF TWELVE (12) MONTHS.</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
+      <c r="C41" s="2" t="n">
+        <v>45807.59373842592</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>45838.5</v>
+      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-06-06 11:00:00</t>
+          <t>6/6/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2595,11 +2759,15 @@
 TRANSNET NATIONAL PORTS AUTHORITY IN THE PORT OF PORT ELIZABETH.</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
+      <c r="C42" s="2" t="n">
+        <v>45807.57770833333</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>45838.5</v>
+      </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-06-13 12:00:00</t>
+          <t>6/13/2025 12:00:00 PM</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2649,11 +2817,15 @@
           <t>PROVISION FOR THE REPAIRS AND MAINTENANCE OF WHARF FOREMAN FOR CIVIL MAINTENANCE DEPARTMENT AT THE PORT OF RICHARDS BAY FOR A PERIOD OF THREE (03) MONTHS</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
+      <c r="C43" s="2" t="n">
+        <v>45807.52611111111</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>45838.5</v>
+      </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-06-18 10:00:00</t>
+          <t>6/18/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2703,8 +2875,12 @@
           <t>Provision of service for Steelwork Repairs in the Port of East London</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+      <c r="C44" s="2" t="n">
+        <v>45807.41094907407</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
@@ -2753,8 +2929,12 @@
           <t>FOR THE TEST AND REPAIR OF INTERNAL TRACTION TRANSFORMER FAULT AT TURFGROND AT, INFRA KOEDOESPOORT</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+      <c r="C45" s="2" t="n">
+        <v>45807.3596875</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>45819.41666666666</v>
+      </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
@@ -2803,8 +2983,12 @@
           <t>MAINTENANCE OF RAILWAY TRACK WITH ON-TRACK MEDIUM PRODUCTION UNIVERAL BALLAST TAMPING MACHINES AND A BALLAST STABILISER COUNTRYWIDE ON AN 'AS AND WHEN” REQUIRED' BASIS</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="C46" s="2" t="n">
+        <v>45807.33966435185</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>45821.41666666666</v>
+      </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
@@ -2854,8 +3038,12 @@
 PROVIDE, SERV;RECERTIFY,XB SAMPLE TEST</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+      <c r="C47" s="2" t="n">
+        <v>45806.6893287037</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>45820.75</v>
+      </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
@@ -2904,11 +3092,15 @@
           <t xml:space="preserve">REPAIR OF THE BOOM HYDRAULIC RAM 524 FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS AT THE DURBAN CONTAINER TERMINAL </t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="C48" s="2" t="n">
+        <v>45806.63712962963</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-06-02 10:00:00</t>
+          <t>6/2/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2958,11 +3150,15 @@
           <t>REPLACEMENT AND INSTALLATION OF FENCE AT THE PORT OF NGQURA AND COEGA KOP QUARRY FOR A PERIOD OF TEN (10) MONTH</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
+      <c r="C49" s="2" t="n">
+        <v>45806.62247685185</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>45838.625</v>
+      </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-06-11 10:00:00</t>
+          <t>6/11/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -3012,11 +3208,15 @@
           <t>REQUEST FOR PROVISION OF SERVICE TO SUPPLY AND DELIVER RO PLANT HIGH PRESSURE FEED PUMP.</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+      <c r="C50" s="2" t="n">
+        <v>45806.55134259259</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>45812.83333333334</v>
+      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-06-02 11:00:00</t>
+          <t>6/2/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3068,11 +3268,15 @@
 TRACTION SUBSTATIONS UNDER THE CONTROL OF DEPOT ENGINEER.</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="C51" s="2" t="n">
+        <v>45806.51459490741</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>45821.41666666666</v>
+      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-06-06 10:00:00</t>
+          <t>6/6/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3122,11 +3326,15 @@
           <t>HEALTH AND SAFETY AGENT/S ON THE PORT ELIZABETH (PE) FOR CIVIL BULK INFRASTRUCTURE UPGRADE (FOR A PERIOD OF THIRTY-SIX (36) MONTHS) AND/OR MARINE INFRASTRUCTURE UPGRADE (FOR A PERIOD OF TWENTY-FOUR (24) MONTHS) AND/OR NATIONAL FIRE SERVICES INFRASTRUCTURE EQUIPMENT UPGRADE PHASE 2A  (FOR A PERIOD OF FIFTEEN (15) MONTHS)</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="C52" s="2" t="n">
+        <v>45806.48064814815</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>45827.5</v>
+      </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-06-05 10:00:00</t>
+          <t>6/5/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -3176,11 +3384,15 @@
           <t>THE APPOINTMENT OF A PROFESSIONAL SERVICE PROVIDER FOR THE BOEGOEBAAI PORT AND RAIL DEVELOPMENT MARKET RESEARCH STUDIES FOR A PERIOD OF SIX (6) MONTHS</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+      <c r="C53" s="2" t="n">
+        <v>45806.45256944445</v>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>45835.66666666666</v>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-06-06 10:00:00</t>
+          <t>6/6/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3230,11 +3442,15 @@
           <t>FOR THE PROVISION OF REPAIRS TO WASH BAY ROOF &amp; HAULER WORKSHOP BUILDING</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="C54" s="2" t="n">
+        <v>45806.4412962963</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-06-10 10:00:00</t>
+          <t>6/10/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3284,11 +3500,15 @@
           <t>FOR THE SUPPLY AND DELIVERY OF XV, XN AND XB WAGONS SAFETY RELIEF VALVES FOR TRANSNET ENGINEERING, FOR GERMISTON AND BLOEMFONTEIN ON AN “AS AND WHEN” REQUIRED BASIS FOR A PERIOD OF FIVE (5) YEARS</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
+      <c r="C55" s="2" t="n">
+        <v>45806.38208333333</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>45838.66666666666</v>
+      </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-06-11 11:00:00</t>
+          <t>6/11/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3338,11 +3558,15 @@
           <t>RFP REQUEST FOR THE PROVISION OF DRY DOCK MAINTENANCE OF THE LAUNCH KITE, PILOT BOAT AVOCET, WORK BOAT CRESTED TERN, TUG OSPREY, TUG CORMORANT, TUG JUTTEN/LOTHENI AND TUG CHARDONNAY FOR TRANSNET NATIONAL PORTS AUTHORITY (TNPA), PORT OF SALDANHA, ON AN AS AND WHEN REQUIRED BASIS FOR A PERIOD OF THIRTY-SIX (36) MONTHS</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
+      <c r="C56" s="2" t="n">
+        <v>45806.37510416667</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>45832.58333333334</v>
+      </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-06-10 11:00:00</t>
+          <t>6/10/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -3392,11 +3616,15 @@
           <t>For an appointment of a publishing house to wholly develop, publish, print and distribute one Magazine for a period of (3) Three years</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
+      <c r="C57" s="2" t="n">
+        <v>45805.73349537037</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>45826.5</v>
+      </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-06-05 11:00:00</t>
+          <t>6/5/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3446,11 +3674,15 @@
           <t>For the Provision of Roof Repairs and General Building Maintenance Services at the ex-Transtel building at TNPA in the Port of Richards Bay for a period of four (4) months.</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" s="2" t="n">
+        <v>45805.58128472222</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>45820.5</v>
+      </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-06-05 10:00:00</t>
+          <t>6/5/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3500,8 +3732,12 @@
           <t>LAB CONSUMABLES</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" s="2" t="n">
+        <v>45805.36445601852</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>45818.625</v>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
@@ -3550,8 +3786,12 @@
           <t>LAB MACHINE MAINTENANCE SERVICES</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
+      <c r="C60" s="2" t="n">
+        <v>45805.36417824074</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>45814.625</v>
+      </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
@@ -3600,11 +3840,15 @@
           <t>PROVISION OF OFFICE, BUILDING, WORKSHOP CLEANING AND TEA SERVICES FOR TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE PORT OF DURBAN: MPT POINT, CAR TERMINAL, MAYDON WHARF AND AGRIBULK FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="C61" s="2" t="n">
+        <v>45804.70929398148</v>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>45819.41666666666</v>
+      </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-06-03 10:00:00</t>
+          <t>6/3/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -3655,8 +3899,12 @@
 EQUIPMENTS AND WELDER CERTIFICATION AT TRANSNET ENGINEERING, GERMISTON.</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="C62" s="2" t="n">
+        <v>45804.65201388889</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>45812.625</v>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
@@ -3705,8 +3953,12 @@
           <t>FOR THE PROVISION OF REPAIR, TESTING AND COMMISSIONING OF TWO RAIL-ROAD SHUNTING LOCOMOTIVES SALDANHA AT TRANSNET ENGINEERING FOR A ONCE-OFF PERIOD</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="C63" s="2" t="n">
+        <v>45804.58878472223</v>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>45833.45833333334</v>
+      </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
@@ -3757,8 +4009,12 @@
 CONVEYOR</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="C64" s="2" t="n">
+        <v>45804.47309027778</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>45818.66666666666</v>
+      </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
@@ -3807,8 +4063,12 @@
           <t>EXPRESSION OF INTEREST (EOI) REQUIRED IN RELATION TO TRIDEM AXLE BOGIE WITH OVERSLUNG SUSPENSION (TRAILER) FOR USE AT PORT TERMINAL, MARITIME BUSINESS, TRANSNET ENGINEERING, RICHARDS BAY.</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+      <c r="C65" s="2" t="n">
+        <v>45804.37309027778</v>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>45819.58333333334</v>
+      </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
@@ -3858,11 +4118,15 @@
 INFRASTRUCTURE MANAGER’S SECURITY DEPARTMENT.</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="C66" s="2" t="n">
+        <v>45804.32800925926</v>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>45832.54166666666</v>
+      </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-06-03 11:00:00</t>
+          <t>6/3/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3912,11 +4176,15 @@
           <t xml:space="preserve"> PROVISION TO REFURBISHMENT OF SUBSTATION 1A AND 1B AT NGQURA CONTAINER TERMINAL FOR TRANSNET SOC LTD (REG NO:1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED AS “TPT”) FOR NGQURA CONTAINER TERMINAL AS A ONCE OFF </t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="C67" s="2" t="n">
+        <v>45803.6796875</v>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>45835.58333333334</v>
+      </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-06-10 11:00:00</t>
+          <t>6/10/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3968,8 +4236,12 @@
 MUNCHER</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+      <c r="C68" s="2" t="n">
+        <v>45803.63376157408</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>45817.66666666666</v>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
@@ -4018,11 +4290,15 @@
           <t>SUPPLY, INSTALLATION, COMMISSIONING AND TESTING OF NEW SMALL BASIC MINI-CNC LATHE MACHINE FOR PD BUSINESS AT KOEDOESPOORT FOR ONCE OFF PERIOD, AT TRANSNET ENGINEERING</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
+      <c r="C69" s="2" t="n">
+        <v>45803.56710648148</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>45813.58333333334</v>
+      </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-30 10:00:00</t>
+          <t>5/30/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -4076,11 +4352,15 @@
 </t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
+      <c r="C70" s="2" t="n">
+        <v>45803.54571759259</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>45813.5</v>
+      </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-29 10:00:00</t>
+          <t>5/29/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4130,8 +4410,12 @@
           <t>FOR THE SUPPLY, DELIVERY AND INSTALLATION OF STEEL PALISADE WITH ELECTRIC FENCE AT OGIES/ERMELO</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="C71" s="2" t="n">
+        <v>45803.47934027778</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>45817.41666666666</v>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
@@ -4180,11 +4464,15 @@
           <t>PROVISION OF HYGIENE AND PEST CONTROL SERVICES AT SCHEEPERSNECK FOR 24 MONTHS PERIOD</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="C72" s="2" t="n">
+        <v>45803.36966435185</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>45813.45833333334</v>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-30 11:00:00</t>
+          <t>5/30/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4234,8 +4522,12 @@
           <t xml:space="preserve">FOR THE MAINTENANCE OF RAILWAY TRACK WITH AN ON-TRACK HIGH PRODUCTION SCREENING MACHINE ON ALL LINES OWNED AND MAINTAINED BY TRANSNET </t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
+      <c r="C73" s="2" t="n">
+        <v>45803.32575231481</v>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
@@ -4284,8 +4576,12 @@
           <t>PROVISION OF COMPREHENSIVE SCAFFOLDING SERVICES ON AN AS AND WHEN REQUIRED BASIS FOR A PERIOD OF 2 MONTHS FOR TRANSNET PORT TERMINALS RICHARDS BAY</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+      <c r="C74" s="2" t="n">
+        <v>45800.67446759259</v>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>45814.58333333334</v>
+      </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
@@ -4335,8 +4631,12 @@
 RECON, COMP;DRAWGEAR KEYSTONE</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
+      <c r="C75" s="2" t="n">
+        <v>45800.63063657407</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>45818.75</v>
+      </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
@@ -4385,11 +4685,15 @@
           <t>FOR THE PROVISION OF MAINTENANCE FOR RAIL DISPATCH BUILDING TARLTON DEPOT ON A ONCE OFF BASIS</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
+      <c r="C76" s="2" t="n">
+        <v>45800.53383101852</v>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>45817.66666666666</v>
+      </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-06-02 11:00:00</t>
+          <t>6/2/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4440,8 +4744,12 @@
 </t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
+      <c r="C77" s="2" t="n">
+        <v>45800.5280324074</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
@@ -4490,11 +4798,15 @@
           <t xml:space="preserve">PROVISION OF S04 TAIL STRUCTURAL REPAIRS </t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
+      <c r="C78" s="2" t="n">
+        <v>45800.51077546296</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>45814.33333333334</v>
+      </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-30 10:00:00</t>
+          <t>5/30/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -4544,8 +4856,12 @@
           <t>FOR THE SUPPLY AND DELIVERY OF SOAPS AND DETERGENTS TRANSNET SOC LTD REG. NO. 1990/000900) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) FOR THE DURBAN CONTAINER TERMINALS PIER 1 AND PIER 2. FOR A PERIOD OF THIRTY-SIX MONTHS (36) MONTHS.</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr"/>
+      <c r="C79" s="2" t="n">
+        <v>45800.50451388889</v>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>45817.5</v>
+      </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
@@ -4594,8 +4910,12 @@
           <t>THE PROVISION OF AN ACCREDITED YOUNG LEADERS PROGRAMME WITHIN TRANSNET, FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="C80" s="2" t="n">
+        <v>45800.47005787037</v>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>45835.66666666666</v>
+      </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
@@ -4644,11 +4964,15 @@
           <t>REPAIR DAMAGED LEAKING ROOFS WITHIN THE RM BUSINESS WORKSHOP 150 EEL ROAD UMBILO</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="C81" s="2" t="n">
+        <v>45800.44152777778</v>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>45817.54166666666</v>
+      </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-06-03 11:00:00</t>
+          <t>6/3/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -4698,11 +5022,15 @@
           <t>FOR THE PROVISION OF WASTE REMOVAL SERVICES IN NORTHERN KZN (EMPANGENI, RICHARDS BAY AND VRYHEID AND SURROUNDING AREAS) FOR TRANSNET PROPERTY FOR A PERIOD OF THIRTY SIX (36) MONTHS</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+      <c r="C82" s="2" t="n">
+        <v>45799.79829861111</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-29 09:30:00</t>
+          <t>5/29/2025 9:30:00 AM</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -4752,11 +5080,15 @@
           <t xml:space="preserve">PROVISION OF PEST CONTROL SERVICES AT VRYHEID, EMPANGENI , RICHARDS BAY AND SURROUNDING AREAS FOR TRANSNET PROPERTY FOR A PERIOD OF 36 MONTHS. </t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr"/>
+      <c r="C83" s="2" t="n">
+        <v>45799.79804398148</v>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>45821.58333333334</v>
+      </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-29 11:00:00</t>
+          <t>5/29/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -4806,11 +5138,15 @@
           <t>FOR THE APPOINTMENT OF A SERVICE PROVIDER TO CONDUCT INTERNAL SHOTBLAST FOR RAIL TANKS AT TRANSNET ENGINEERING, GERMISTON DEPOT ON AN AS AND WHEN BASIS FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
+      <c r="C84" s="2" t="n">
+        <v>45799.65636574074</v>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>45813.66666666666</v>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-29 11:00:00</t>
+          <t>5/29/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -4860,11 +5196,15 @@
           <t>SUPPLY, INSTALLATION AND MOULDING HDPE PIPES FOR INTERMEDIATE PUMPS FOR TRANSNET PORT TERMINAL - RICHARDS BAY - AS A ONCE OFF SERVICE</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
+      <c r="C85" s="2" t="n">
+        <v>45799.50821759259</v>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>45814.58333333334</v>
+      </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-30 11:00:00</t>
+          <t>5/30/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -4914,11 +5254,15 @@
           <t>THE PROVISION OF INSPECTION AND CALIBRATION SERVICES FOR PRESSURE RELIEF DEVICES AT VARIOUS TRANSNET PIPELINES SITES FOR A PERIOD OF FOUR (4) YEARS.</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr"/>
+      <c r="C86" s="2" t="n">
+        <v>45798.73452546296</v>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>45814.5</v>
+      </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-30 10:00:00</t>
+          <t>5/30/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4968,8 +5312,12 @@
           <t>FOR THE APPOINTMENT OF FINANCIAL INSTITUTION(S) TO ACT AS LEAD ARRANGER(S) AND TRANSACTION ADVISOR(S) FOR SPECIFIC ISSUANCES UNDER TRANSNET’S R80 BILLION DOMESTIC MEDIUM-TERM NOTE (“DMTN”) PROGRAMME FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr"/>
+      <c r="C87" s="2" t="n">
+        <v>45798.68741898148</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>45821.66666666666</v>
+      </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
@@ -5018,8 +5366,12 @@
           <t>Provision of service for the maintenance, repair and installation (if necessary) of air conditioning units in Kimberley South relay rooms (Spuitfontein to De Aar) as and when required for a period of two (2) years.</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="C88" s="2" t="n">
+        <v>45798.6144212963</v>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>45825.41666666666</v>
+      </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
@@ -5069,8 +5421,12 @@
 </t>
         </is>
       </c>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
+      <c r="C89" s="2" t="n">
+        <v>45797.47945601852</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
@@ -5119,11 +5475,15 @@
           <t xml:space="preserve"> CIDB - FOR THE PROVISION TO REPAIR THE CONCRETE STRUCTURE FOR GP4 SHED FOR TRANSNET SOC LTD</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
+      <c r="C90" s="2" t="n">
+        <v>45796.62003472223</v>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>45814.54166666666</v>
+      </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2025-05-26 10:00:00</t>
+          <t>5/26/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -5175,11 +5535,15 @@
 </t>
         </is>
       </c>
-      <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr"/>
+      <c r="C91" s="2" t="n">
+        <v>45794.54615740741</v>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>45812.58333333334</v>
+      </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2025-05-19 11:00:00</t>
+          <t>5/19/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -5229,11 +5593,15 @@
           <t>FOR THE SUPPLY, DELIVERY, INSTALLATION, TESTING AND COMMISSIONING OF 9 OFF ROTARY SCREW TYPE COMPRESSORS AND AIR DRYERS FOR TRANSNET ENGINEERING AT VARIOUS CORRIDOR DEPOTS (NORTH CAPE AND CONTAINER CORRIDORS)</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr"/>
+      <c r="C92" s="2" t="n">
+        <v>45793.60487268519</v>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>45818.5</v>
+      </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2025-05-26 09:30:00</t>
+          <t>5/26/2025 9:30:00 AM</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -5283,11 +5651,15 @@
           <t>FOR THE PROVISION OF NETWORK DETECTION AND RESPONSE (NDR) SOLUTION FOR A PERIOD OF THREE (3) YEARS.</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="C93" s="2" t="n">
+        <v>45793.48670138889</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>45827.5</v>
+      </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>2025-05-23 11:00:00</t>
+          <t>5/23/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5338,11 +5710,15 @@
 </t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="C94" s="2" t="n">
+        <v>45792.64659722222</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>45838.75</v>
+      </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2025-05-27 10:00:00</t>
+          <t>5/27/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -5392,11 +5768,15 @@
           <t>SUPPLY AND DELIVERY OF VARIOUS AMOUR ROCK FOR THE CONSTRUCTION WORK IN THE UPGRADE OF THE BREAKWATERS (NEW DOLOSSE) AT THE PORT OF RICHARDS BAY</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
+      <c r="C95" s="2" t="n">
+        <v>45792.61826388889</v>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>45817.66666666666</v>
+      </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>2025-05-26 10:00:00</t>
+          <t>5/26/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -5446,11 +5826,15 @@
           <t>THE ESTABLISHMENT OF AN  APPROVED LIST OF SERVICE PROVIDERS FOR PROVISION OF LEGAL SERVICES FOR A PERIOD OF FIVE (5) YEARS</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
+      <c r="C96" s="2" t="n">
+        <v>45791.66534722222</v>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>45825.5</v>
+      </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>2024-05-23 11:00:00</t>
+          <t>5/23/2024 11:00:00 AM</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -5501,11 +5885,15 @@
 </t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
+      <c r="C97" s="2" t="n">
+        <v>45791.47337962963</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>45821.75</v>
+      </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>2025-05-19 13:00:00</t>
+          <t>5/19/2025 1:00:00 PM</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -5559,11 +5947,15 @@
 </t>
         </is>
       </c>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
+      <c r="C98" s="2" t="n">
+        <v>45790.86484953704</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>45814.41666666666</v>
+      </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2025-05-22 10:00:00</t>
+          <t>5/22/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -5613,11 +6005,15 @@
           <t>FOR THE DESIGN, MANUFACTURE, OFF SITE TESTING, SUPPLY, DELIVERY, INSTALLATION, TESTING AND COMMISSIONING OF ONE (1) NEW 1000KVA MINI SUBSTATION AND ONE (1) 1000KVA MOBILE GENERATOR FOR THE ENGINEERING EQUIPMENT SERVICES (EES) BUILDING, FOR TRANSNET SOC LTD OPERATING AS TRANSNET PORT TERMINALS, (HEREINAFTER REFERRED TO AS “TPT”), AT DURBAN CONTAINER TERMINAL PIER 1, FOR THE DURATION OF 12 MONTHS</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
+      <c r="C99" s="2" t="n">
+        <v>45790.62701388889</v>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>45817</v>
+      </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2025-05-21 00:00:00</t>
+          <t>5/21/2025 12:00:00 AM</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -5667,11 +6063,15 @@
           <t>MECHANICAL UPGRADE AT SASOLBURG DIESEL STORAGE DEPOT, FREE STATE.</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="C100" s="2" t="n">
+        <v>45789.69364583334</v>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>45821.41666666666</v>
+      </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>2025-05-22 10:12:00</t>
+          <t>5/22/2025 10:12:00 AM</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -5721,11 +6121,15 @@
           <t xml:space="preserve">THE DESIGN, SUPPLY, DELIVERY, INSTALLATION, TESTING AND COMMISSIONING OF A COMPLETE NEW SHOT BLAST BOOTH INCLUDING THE STRUCTURE FOR THE LOCOMOTIVE BUSINESS DURBAN FOR A PERIOD OF FOUR (04) MONTHS. </t>
         </is>
       </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="C101" s="2" t="n">
+        <v>45786.61042824074</v>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>45814.75</v>
+      </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>2025-05-19 11:00:00</t>
+          <t>5/19/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -5775,8 +6179,12 @@
           <t>FOR A SERVICE PROVIDER TO PROVIDE THE SERVICES OF AN APPROVED INSPECTION AUTHORITY (AIA) TO CONDUCT SAMPLE TESTING ON THE XB WAGONS FLEET IN LINE WITH SPECIFICATION EW_KLP_SPEC_2003 IN BLOEMFONTEIN ON AN “AS AND WHEN” REQUIRED BASIS FOR A PERIOD OF FOUR (4) YEARS.</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+      <c r="C102" s="2" t="n">
+        <v>45785.36899305556</v>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>45814.66666666666</v>
+      </c>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr">
         <is>
@@ -5825,11 +6233,15 @@
           <t>FOR AN APPOINTMENT OF A SERVICE PROVIDER TO OPERATE  AND  TAKE OVER OWNERSHIP SCHOOL OF EXCELLENCE</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
+      <c r="C103" s="2" t="n">
+        <v>45784.35107638889</v>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>45821.625</v>
+      </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2025-05-21 11:00:00</t>
+          <t>5/21/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -5879,11 +6291,15 @@
           <t>FOR THE APPOINTMENT OF A REGISTERED PROFESSIONAL TO PERFORM AN EPC ASSESSMENT, MEASUREMENT OF THE BUILDING NET FLOOR AREA AND ENERGY DATA ON 13 FACILITIES TO TRANSNET SOC LTD (REG. NO. 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS (HEREINAFTER REFERRED TO AS “TPT”) AT THE VARIOUS TRANSNET PORT TERMINALS ON A ONCE OFF BASIS.</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr"/>
+      <c r="C104" s="2" t="n">
+        <v>45783.49142361111</v>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>45821.5</v>
+      </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2025-05-16 11:00:00</t>
+          <t>5/16/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -5933,11 +6349,15 @@
           <t>DESIGN, SUPPLY, DELIVER AND CONSTRUCT THE PERIMETER FENCE WITH INTRUSION DETECTION AT UITENHAGE (SWARTKOPS), FOR A PERIOD OF 06 MONTHS</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
+      <c r="C105" s="2" t="n">
+        <v>45782.56052083334</v>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>45817.75</v>
+      </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2025-05-13 10:00:00</t>
+          <t>5/13/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -5987,11 +6407,15 @@
           <t>FOR THE LEASE AND/OR DEVELOPMENT OF THE REMAINDER OF ERF 34104 BELLVILLE (UNREGISTERED SUBDIVISION OF REMAINDER OF ERF 11661 BELLVILLE), ERF 34103 BELLVILLE (UNREGISTERED SUBDIVISION OF REMAINDER OF ERF 11659 BELLVILLE), ERF 22933 PAROW.</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
+      <c r="C106" s="2" t="n">
+        <v>45780.34752314815</v>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>45838.95833333334</v>
+      </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2025-05-19 11:00:00</t>
+          <t>5/19/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -6041,11 +6465,15 @@
           <t>DECOMMISSIONING OF OBSOLETE NETWORK VIDEO RECORDERS (NVRs), SUPPLY, INSTALLATION, CONFIGURATION, INTEGRATION, TRAINING, MAINTENANCE, AND COMMISSIONING OF A NEW NVR AND SOFTWARE FOR THE CCTV SURVEILLANCE SYSTEM AT KILNERPARK CORPORATE OFFICE FOR A PERIOD OF 12 MONTHS</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+      <c r="C107" s="2" t="n">
+        <v>45777.94576388889</v>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>45818.41666666666</v>
+      </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>2025-05-14 11:00:00</t>
+          <t>5/14/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -6095,11 +6523,15 @@
           <t>FOR THE SUPPLY, INSTALLATION, AND COMMISSIONING OF SHOP 5 WORKSHOP EQUIPMENT/MACHINERY AT THE DRY BULK TERMINAL PORT OF RICHARDS BAY WORKS FOR TRANSNET SOC LTD OPERATING AS TRANSNET PORT TERMINALS</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
+      <c r="C108" s="2" t="n">
+        <v>45764.48126157407</v>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>45812.5</v>
+      </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>2025-05-06 11:00:00</t>
+          <t>5/6/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -6149,11 +6581,15 @@
           <t>DESIGN, SUPPLY, INSTALLATION (EPC CONTRACTOR) AND PROVIDE PLANNED MAINTENANCE FOR A LIMITED PERIOD FOR THE VAPOUR RECOVERY UNIT SYSTEM AT THE TPL TARLTON PETROLEUM PRODUCTS HANDLING AND BULK STORAGE FACILITY</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr"/>
+      <c r="C109" s="2" t="n">
+        <v>45763.49534722222</v>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>45814.625</v>
+      </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>2025-04-25 11:00:00</t>
+          <t>4/25/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -6203,11 +6639,15 @@
           <t>REQUEST FOR PROPOSALS FOR THE APPOINTMENT OF A TERMINAL OPERATOR TO FINANCE, DESIGN, CONSTRUCT, OPERATE, MAINTAIN, AND TRANSFER A MULTI-PURPOSE TERMINAL HANDLING FRESH PRODUCE AND COMPATIBLE BREAK BULK CARGO FOR A TWENTY-FIVE (25) YEAR CONCESSION PERIOD AT MAYDON WHARF PRECINCT IN THE PORT OF DURBAN.</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr"/>
+      <c r="C110" s="2" t="n">
+        <v>45758.65010416666</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>45898.66666666666</v>
+      </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>2025-05-07 10:00:00</t>
+          <t>5/7/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -6257,11 +6697,15 @@
           <t>Request for Qualification (RFQ) for the Establishment of the Rolling Stock Leasing Company (LeaseCo) for Transnet SOC Ltd operating as Transnet Corporate Centre</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr"/>
+      <c r="C111" s="2" t="n">
+        <v>45755.66251157408</v>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>45842.66666666666</v>
+      </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2025-05-06 11:00:00</t>
+          <t>5/6/2025 11:00:00 AM</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -6311,11 +6755,15 @@
           <t>APPOINTMENT OF A TERMINAL OPERATOR TO ACQUIRE, OPERATE, MAINTAIN, REFURBISH, AND/OR CONSTRUCT AND TRANSFER A LIQUID BULK TERMINAL FOR A TWENTY-FIVE (25) YEAR CONCESSION PERIOD AT THE PORT OF CAPE TOWN LIQUID BULK PRECINCT</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr"/>
+      <c r="C112" s="2" t="n">
+        <v>45750.64232638889</v>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>45881.66666666666</v>
+      </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2025-04-17 10:00:00</t>
+          <t>4/17/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -6366,11 +6814,15 @@
 CONVEYOR SOLUTION FOR TRANSNET SOC (REG. N0 1990/000900/30) OPERATING AS TRANSNET PORT TERMINALS RICHARDS BAY (HEREINAFTER REFERRED TO AS “TPT RCB”)</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
+      <c r="C113" s="2" t="n">
+        <v>45743.61306712963</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>45838.41666666666</v>
+      </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2025-04-10 10:00:00</t>
+          <t>4/10/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -6420,11 +6872,15 @@
           <t>REQUEST FOR PROPOSAL FOR THE APPOINTMENT OF A TERMINAL OPERATOR TO FINANCE, DESIGN, CONSTRUCT, OPERATE, MAINTAIN, AND TRANSFER A MULTI-PURPOSE TERMINAL HANDLING AGRICULTURAL DRY BULK AND OTHER COMPATIBLE CARGO FOR A TWENTY-FIVE (25) YEAR CONCESSION PERIOD AT MAYDON WHARF PRECINCT AT THE PORT OF DURBAN.</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr"/>
+      <c r="C114" s="2" t="n">
+        <v>45723.59657407407</v>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>45849.66666666666</v>
+      </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2025-03-27 10:00:00</t>
+          <t>3/27/2025 10:00:00 AM</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">

</xml_diff>